<commit_message>
Fixed incx instruction description and added jump instruction definition
</commit_message>
<xml_diff>
--- a/microcode/microcode.xlsx
+++ b/microcode/microcode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faust\Documents\Programming\retro-cpu\microcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037BEAFE-6A8E-4F0D-A964-C2B5FC001487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57294C6-7017-4E39-B562-C411D8C355B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14865" yWindow="3960" windowWidth="21585" windowHeight="13725" xr2:uid="{6E1463FF-F293-475C-B9F6-92700082F5EB}"/>
+    <workbookView xWindow="705" yWindow="3240" windowWidth="19950" windowHeight="13725" xr2:uid="{6E1463FF-F293-475C-B9F6-92700082F5EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="83">
   <si>
     <t>I0</t>
   </si>
@@ -296,6 +296,15 @@
   </si>
   <si>
     <t>INCYStep3</t>
+  </si>
+  <si>
+    <t>I4</t>
+  </si>
+  <si>
+    <t>INCZStep2</t>
+  </si>
+  <si>
+    <t>INCZStep3</t>
   </si>
 </sst>
 </file>
@@ -568,7 +577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -645,6 +654,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -686,6 +698,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1008,39 +1023,39 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15E04F54-319B-4A29-A4E0-3412CD7198C4}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:BE23"/>
+  <dimension ref="A1:BF25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S23" sqref="S23"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="27" width="5.28515625" customWidth="1"/>
-    <col min="28" max="32" width="4.7109375" customWidth="1"/>
-    <col min="33" max="33" width="16.140625" customWidth="1"/>
-    <col min="34" max="34" width="15.85546875" customWidth="1"/>
-    <col min="35" max="35" width="28.140625" customWidth="1"/>
-    <col min="36" max="36" width="14" customWidth="1"/>
-    <col min="37" max="37" width="16.7109375" customWidth="1"/>
-    <col min="38" max="38" width="19" customWidth="1"/>
-    <col min="40" max="40" width="31.140625" customWidth="1"/>
-    <col min="42" max="42" width="21.7109375" customWidth="1"/>
-    <col min="43" max="43" width="18.85546875" customWidth="1"/>
-    <col min="44" max="51" width="20.7109375" customWidth="1"/>
-    <col min="52" max="52" width="24.140625" customWidth="1"/>
-    <col min="54" max="56" width="14.42578125" customWidth="1"/>
-    <col min="57" max="57" width="77.85546875" customWidth="1"/>
+    <col min="5" max="28" width="5.28515625" customWidth="1"/>
+    <col min="29" max="33" width="4.7109375" customWidth="1"/>
+    <col min="34" max="34" width="16.140625" customWidth="1"/>
+    <col min="35" max="35" width="15.85546875" customWidth="1"/>
+    <col min="36" max="36" width="28.140625" customWidth="1"/>
+    <col min="37" max="37" width="14" customWidth="1"/>
+    <col min="38" max="38" width="16.7109375" customWidth="1"/>
+    <col min="39" max="39" width="19" customWidth="1"/>
+    <col min="41" max="41" width="31.140625" customWidth="1"/>
+    <col min="43" max="43" width="21.7109375" customWidth="1"/>
+    <col min="44" max="44" width="18.85546875" customWidth="1"/>
+    <col min="45" max="52" width="20.7109375" customWidth="1"/>
+    <col min="53" max="53" width="24.140625" customWidth="1"/>
+    <col min="55" max="57" width="14.42578125" customWidth="1"/>
+    <col min="58" max="58" width="77.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:58" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>49</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -1050,163 +1065,166 @@
         <v>24</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AH1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AI1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AK1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AL1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AM1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AN1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AO1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AO1" s="7" t="s">
+      <c r="AP1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AP1" s="7" t="s">
+      <c r="AQ1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AQ1" s="25" t="s">
+      <c r="AR1" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="AR1" s="26" t="s">
+      <c r="AS1" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="AS1" s="26" t="s">
+      <c r="AT1" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="AT1" s="26" t="s">
+      <c r="AU1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="AU1" s="26" t="s">
+      <c r="AV1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="AV1" s="26" t="s">
+      <c r="AW1" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="AW1" s="26" t="s">
+      <c r="AX1" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="AX1" s="26" t="s">
+      <c r="AY1" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="AY1" s="26" t="s">
+      <c r="AZ1" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="AZ1" s="26" t="s">
+      <c r="BA1" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="BB1" s="6" t="s">
+      <c r="BC1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="BC1" s="6" t="s">
+      <c r="BD1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="BD1" s="6" t="s">
+      <c r="BE1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="BE1" s="6" t="s">
+      <c r="BF1" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:57" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:58" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>37</v>
       </c>
@@ -1222,38 +1240,38 @@
       <c r="E2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="28" t="s">
         <v>48</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="13">
-        <v>0</v>
-      </c>
-      <c r="J2" s="29">
-        <v>0</v>
-      </c>
-      <c r="K2" s="14">
-        <v>0</v>
-      </c>
-      <c r="L2" s="15">
-        <v>0</v>
-      </c>
-      <c r="M2" s="16">
-        <v>0</v>
-      </c>
-      <c r="N2" s="17">
+      <c r="H2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="13">
+        <v>0</v>
+      </c>
+      <c r="K2" s="30">
+        <v>0</v>
+      </c>
+      <c r="L2" s="14">
+        <v>0</v>
+      </c>
+      <c r="M2" s="15">
+        <v>0</v>
+      </c>
+      <c r="N2" s="16">
         <v>0</v>
       </c>
       <c r="O2" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q2" s="17">
         <v>0</v>
@@ -1280,10 +1298,10 @@
         <v>0</v>
       </c>
       <c r="Y2" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z2" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA2" s="17">
         <v>0</v>
@@ -1291,7 +1309,7 @@
       <c r="AB2" s="17">
         <v>0</v>
       </c>
-      <c r="AC2" s="16">
+      <c r="AC2" s="17">
         <v>0</v>
       </c>
       <c r="AD2" s="16">
@@ -1303,47 +1321,47 @@
       <c r="AF2" s="16">
         <v>0</v>
       </c>
-      <c r="AG2" s="22" t="str">
-        <f>_xlfn.CONCAT(M2:V2)</f>
+      <c r="AG2" s="16">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="22" t="str">
+        <f>_xlfn.CONCAT(N2:W2)</f>
         <v>0010000000</v>
       </c>
-      <c r="AH2" s="22" t="str">
-        <f>_xlfn.CONCAT(W2:AF2)</f>
+      <c r="AI2" s="22" t="str">
+        <f>_xlfn.CONCAT(X2:AG2)</f>
         <v>0010000000</v>
       </c>
-      <c r="AI2" s="22" t="str">
-        <f>_xlfn.CONCAT(AG2:AH2)</f>
+      <c r="AJ2" s="22" t="str">
+        <f>_xlfn.CONCAT(AH2:AI2)</f>
         <v>00100000000010000000</v>
       </c>
-      <c r="AJ2" s="23" t="str">
-        <f>_xlfn.CONCAT(B2:L2)</f>
-        <v>*******0000</v>
-      </c>
-      <c r="AK2" s="23" t="e">
-        <f>BIN2HEX(AJ2,5)</f>
+      <c r="AK2" s="23" t="str">
+        <f>_xlfn.CONCAT(B2:M2)</f>
+        <v>********0000</v>
+      </c>
+      <c r="AL2" s="23" t="e">
+        <f>BIN2HEX(AK2,5)</f>
         <v>#NUM!</v>
       </c>
-      <c r="AL2" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL2" ca="1">MY_BIN2HEX(AI2)</f>
+      <c r="AM2" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM2" ca="1">MY_BIN2HEX(AJ2)</f>
         <v>#NAME?</v>
       </c>
-      <c r="AM2" s="9" t="s">
+      <c r="AN2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="AN2" s="24" t="s">
+      <c r="AO2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="AO2" s="9" t="s">
+      <c r="AP2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="AP2" s="27" t="s">
+      <c r="AQ2" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="AQ2" s="23" t="s">
+      <c r="AR2" s="23" t="s">
         <v>6</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="AS2" s="1" t="s">
         <v>35</v>
@@ -1369,20 +1387,23 @@
       <c r="AZ2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="BB2" s="8" t="s">
+      <c r="BA2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="BC2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="BC2" s="8" t="s">
+      <c r="BD2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="BD2" s="31" t="s">
+      <c r="BE2" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="BE2" s="30" t="s">
+      <c r="BF2" s="31" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:57" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:58" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>36</v>
       </c>
@@ -1398,35 +1419,35 @@
       <c r="E3" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="28" t="s">
         <v>48</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="13">
-        <v>0</v>
-      </c>
-      <c r="J3" s="29">
-        <v>0</v>
-      </c>
-      <c r="K3" s="14">
-        <v>0</v>
-      </c>
-      <c r="L3" s="15">
-        <v>1</v>
-      </c>
-      <c r="M3" s="19">
-        <v>0</v>
-      </c>
-      <c r="N3" s="20">
-        <v>1</v>
+      <c r="H3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="13">
+        <v>0</v>
+      </c>
+      <c r="K3" s="30">
+        <v>0</v>
+      </c>
+      <c r="L3" s="14">
+        <v>0</v>
+      </c>
+      <c r="M3" s="15">
+        <v>1</v>
+      </c>
+      <c r="N3" s="19">
+        <v>0</v>
       </c>
       <c r="O3" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" s="20">
         <v>0</v>
@@ -1450,10 +1471,10 @@
         <v>0</v>
       </c>
       <c r="W3" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X3" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y3" s="20">
         <v>0</v>
@@ -1462,10 +1483,10 @@
         <v>0</v>
       </c>
       <c r="AA3" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB3" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC3" s="20">
         <v>0</v>
@@ -1476,39 +1497,42 @@
       <c r="AE3" s="20">
         <v>0</v>
       </c>
-      <c r="AF3" s="21">
-        <v>1</v>
-      </c>
-      <c r="AG3" s="22" t="str">
-        <f t="shared" ref="AG3:AG12" si="0">_xlfn.CONCAT(M3:V3)</f>
+      <c r="AF3" s="20">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="21">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="22" t="str">
+        <f t="shared" ref="AH3:AH12" si="0">_xlfn.CONCAT(N3:W3)</f>
         <v>0100000000</v>
       </c>
-      <c r="AH3" s="22" t="str">
-        <f t="shared" ref="AH3:AH15" si="1">_xlfn.CONCAT(W3:AF3)</f>
+      <c r="AI3" s="22" t="str">
+        <f t="shared" ref="AI3:AI15" si="1">_xlfn.CONCAT(X3:AG3)</f>
         <v>1000100001</v>
       </c>
-      <c r="AI3" s="22" t="str">
-        <f t="shared" ref="AI3:AI15" si="2">_xlfn.CONCAT(AG3:AH3)</f>
+      <c r="AJ3" s="22" t="str">
+        <f t="shared" ref="AJ3:AJ15" si="2">_xlfn.CONCAT(AH3:AI3)</f>
         <v>01000000001000100001</v>
       </c>
-      <c r="AJ3" s="23" t="str">
-        <f>_xlfn.CONCAT(B3:L3)</f>
-        <v>*******0001</v>
-      </c>
-      <c r="AK3" s="23" t="e">
-        <f t="shared" ref="AK3:AK5" si="3">BIN2HEX(AJ3,5)</f>
+      <c r="AK3" s="23" t="str">
+        <f>_xlfn.CONCAT(B3:M3)</f>
+        <v>********0001</v>
+      </c>
+      <c r="AL3" s="23" t="e">
+        <f t="shared" ref="AL3:AL5" si="3">BIN2HEX(AK3,5)</f>
         <v>#NUM!</v>
       </c>
-      <c r="AL3" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL3" ca="1">MY_BIN2HEX(AI3)</f>
+      <c r="AM3" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM3" ca="1">MY_BIN2HEX(AJ3)</f>
         <v>#NAME?</v>
       </c>
-      <c r="AM3" s="23"/>
-      <c r="AN3" s="24"/>
+      <c r="AN3" s="23"/>
       <c r="AO3" s="24"/>
       <c r="AP3" s="24"/>
+      <c r="AQ3" s="24"/>
     </row>
-    <row r="4" spans="1:57" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:58" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>50</v>
       </c>
@@ -1518,37 +1542,37 @@
       <c r="C4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E4" s="10">
         <v>0</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="28">
         <v>0</v>
       </c>
       <c r="G4" s="11">
         <v>0</v>
       </c>
-      <c r="H4" s="28">
-        <v>1</v>
-      </c>
-      <c r="I4" s="13">
-        <v>0</v>
-      </c>
-      <c r="J4" s="29">
-        <v>0</v>
-      </c>
-      <c r="K4" s="14">
-        <v>1</v>
-      </c>
-      <c r="L4" s="15">
-        <v>0</v>
-      </c>
-      <c r="M4" s="16">
-        <v>0</v>
-      </c>
-      <c r="N4" s="17">
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+      <c r="I4" s="29">
+        <v>1</v>
+      </c>
+      <c r="J4" s="13">
+        <v>0</v>
+      </c>
+      <c r="K4" s="30">
+        <v>0</v>
+      </c>
+      <c r="L4" s="14">
+        <v>1</v>
+      </c>
+      <c r="M4" s="15">
+        <v>0</v>
+      </c>
+      <c r="N4" s="16">
         <v>0</v>
       </c>
       <c r="O4" s="17">
@@ -1579,13 +1603,13 @@
         <v>0</v>
       </c>
       <c r="X4" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="17">
         <v>1</v>
       </c>
       <c r="Z4" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA4" s="17">
         <v>0</v>
@@ -1602,165 +1626,171 @@
       <c r="AE4" s="17">
         <v>0</v>
       </c>
-      <c r="AF4" s="18">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="22" t="str">
+      <c r="AF4" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="22" t="str">
         <f t="shared" si="0"/>
         <v>0000000000</v>
       </c>
-      <c r="AH4" s="22" t="str">
+      <c r="AI4" s="22" t="str">
         <f t="shared" si="1"/>
         <v>0110000000</v>
       </c>
-      <c r="AI4" s="22" t="str">
+      <c r="AJ4" s="22" t="str">
         <f t="shared" si="2"/>
         <v>00000000000110000000</v>
       </c>
-      <c r="AJ4" s="23" t="str">
-        <f>_xlfn.CONCAT(B4:L4)</f>
-        <v>***00010010</v>
-      </c>
-      <c r="AK4" s="23" t="e">
+      <c r="AK4" s="23" t="str">
+        <f>_xlfn.CONCAT(B4:M4)</f>
+        <v>***000010010</v>
+      </c>
+      <c r="AL4" s="23" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
-      <c r="AL4" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL4" ca="1">MY_BIN2HEX(AI4)</f>
+      <c r="AM4" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM4" ca="1">MY_BIN2HEX(AJ4)</f>
         <v>#NAME?</v>
       </c>
-      <c r="AM4" s="23"/>
-      <c r="AN4" s="24"/>
+      <c r="AN4" s="23"/>
       <c r="AO4" s="24"/>
       <c r="AP4" s="24"/>
+      <c r="AQ4" s="24"/>
     </row>
-    <row r="5" spans="1:57" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:58" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="33">
-        <v>0</v>
-      </c>
-      <c r="F5" s="34">
-        <v>0</v>
-      </c>
-      <c r="G5" s="34">
+      <c r="B5" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="34">
+        <v>0</v>
+      </c>
+      <c r="F5" s="44">
+        <v>0</v>
+      </c>
+      <c r="G5" s="35">
         <v>0</v>
       </c>
       <c r="H5" s="35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="37">
         <v>0</v>
       </c>
       <c r="K5" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" s="39">
         <v>1</v>
       </c>
       <c r="M5" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="41">
         <v>0</v>
       </c>
-      <c r="O5" s="41">
-        <v>0</v>
-      </c>
-      <c r="P5" s="41">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="41">
-        <v>1</v>
-      </c>
-      <c r="R5" s="41">
-        <v>0</v>
-      </c>
-      <c r="S5" s="41">
-        <v>0</v>
-      </c>
-      <c r="T5" s="41">
-        <v>0</v>
-      </c>
-      <c r="U5" s="41">
-        <v>0</v>
-      </c>
-      <c r="V5" s="41">
-        <v>0</v>
-      </c>
-      <c r="W5" s="41">
-        <v>0</v>
-      </c>
-      <c r="X5" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="41">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="41">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="41">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="41">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="40">
+      <c r="O5" s="42">
+        <v>0</v>
+      </c>
+      <c r="P5" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="42">
+        <v>0</v>
+      </c>
+      <c r="R5" s="42">
+        <v>1</v>
+      </c>
+      <c r="S5" s="42">
+        <v>0</v>
+      </c>
+      <c r="T5" s="42">
+        <v>0</v>
+      </c>
+      <c r="U5" s="42">
+        <v>0</v>
+      </c>
+      <c r="V5" s="42">
+        <v>0</v>
+      </c>
+      <c r="W5" s="42">
+        <v>0</v>
+      </c>
+      <c r="X5" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="42">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="42">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="42">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="42">
         <v>0</v>
       </c>
       <c r="AD5" s="41">
         <v>0</v>
       </c>
-      <c r="AE5" s="41">
+      <c r="AE5" s="42">
         <v>0</v>
       </c>
       <c r="AF5" s="42">
-        <v>1</v>
-      </c>
-      <c r="AG5" s="22" t="str">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="43">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="22" t="str">
         <f t="shared" si="0"/>
         <v>0000100000</v>
       </c>
-      <c r="AH5" s="22" t="str">
+      <c r="AI5" s="22" t="str">
         <f t="shared" si="1"/>
         <v>0000100001</v>
       </c>
-      <c r="AI5" s="22" t="str">
+      <c r="AJ5" s="22" t="str">
         <f t="shared" si="2"/>
         <v>00001000000000100001</v>
       </c>
-      <c r="AJ5" s="23" t="str">
-        <f>_xlfn.CONCAT(B5:L5)</f>
-        <v>***00010011</v>
-      </c>
-      <c r="AK5" s="23" t="e">
+      <c r="AK5" s="23" t="str">
+        <f>_xlfn.CONCAT(B5:M5)</f>
+        <v>***000010011</v>
+      </c>
+      <c r="AL5" s="23" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
-      <c r="AL5" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL5" ca="1">MY_BIN2HEX(AI5)</f>
+      <c r="AM5" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM5" ca="1">MY_BIN2HEX(AJ5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="AM5" s="23"/>
-      <c r="AN5" s="24"/>
+      <c r="AN5" s="23"/>
       <c r="AO5" s="24"/>
       <c r="AP5" s="24"/>
+      <c r="AQ5" s="24"/>
     </row>
-    <row r="6" spans="1:57" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:58" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>62</v>
       </c>
@@ -1770,37 +1800,37 @@
       <c r="C6" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E6" s="10">
         <v>0</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="28">
         <v>0</v>
       </c>
       <c r="G6" s="11">
-        <v>1</v>
-      </c>
-      <c r="H6" s="28">
-        <v>0</v>
-      </c>
-      <c r="I6" s="13">
-        <v>0</v>
-      </c>
-      <c r="J6" s="29">
-        <v>0</v>
-      </c>
-      <c r="K6" s="14">
-        <v>1</v>
-      </c>
-      <c r="L6" s="15">
-        <v>0</v>
-      </c>
-      <c r="M6" s="16">
-        <v>0</v>
-      </c>
-      <c r="N6" s="17">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11">
+        <v>1</v>
+      </c>
+      <c r="I6" s="29">
+        <v>0</v>
+      </c>
+      <c r="J6" s="13">
+        <v>0</v>
+      </c>
+      <c r="K6" s="30">
+        <v>0</v>
+      </c>
+      <c r="L6" s="14">
+        <v>1</v>
+      </c>
+      <c r="M6" s="15">
+        <v>0</v>
+      </c>
+      <c r="N6" s="16">
         <v>0</v>
       </c>
       <c r="O6" s="17">
@@ -1831,13 +1861,13 @@
         <v>0</v>
       </c>
       <c r="X6" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y6" s="17">
         <v>1</v>
       </c>
       <c r="Z6" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA6" s="17">
         <v>0</v>
@@ -1854,54 +1884,57 @@
       <c r="AE6" s="17">
         <v>0</v>
       </c>
-      <c r="AF6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="22" t="str">
+      <c r="AF6" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="22" t="str">
         <f t="shared" si="0"/>
         <v>0000000000</v>
       </c>
-      <c r="AH6" s="22" t="str">
+      <c r="AI6" s="22" t="str">
         <f t="shared" si="1"/>
         <v>0110000000</v>
       </c>
-      <c r="AI6" s="22" t="str">
+      <c r="AJ6" s="22" t="str">
         <f t="shared" si="2"/>
         <v>00000000000110000000</v>
       </c>
-      <c r="AJ6" s="23" t="str">
-        <f t="shared" ref="AJ6:AJ8" si="4">_xlfn.CONCAT(B6:L6)</f>
-        <v>***00100010</v>
-      </c>
-      <c r="AL6" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL6" ca="1">MY_BIN2HEX(AI6)</f>
+      <c r="AK6" s="23" t="str">
+        <f>_xlfn.CONCAT(B6:M6)</f>
+        <v>***000100010</v>
+      </c>
+      <c r="AM6" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM6" ca="1">MY_BIN2HEX(AJ6)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="7" spans="1:57" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:58" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="33">
-        <v>0</v>
-      </c>
-      <c r="F7" s="34">
-        <v>0</v>
-      </c>
-      <c r="G7" s="34">
-        <v>1</v>
+      <c r="B7" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="34">
+        <v>0</v>
+      </c>
+      <c r="F7" s="44">
+        <v>0</v>
+      </c>
+      <c r="G7" s="35">
+        <v>0</v>
       </c>
       <c r="H7" s="35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="36">
         <v>0</v>
@@ -1910,93 +1943,96 @@
         <v>0</v>
       </c>
       <c r="K7" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" s="39">
         <v>1</v>
       </c>
       <c r="M7" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="41">
         <v>0</v>
       </c>
-      <c r="O7" s="41">
-        <v>0</v>
-      </c>
-      <c r="P7" s="41">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="41">
-        <v>0</v>
-      </c>
-      <c r="R7" s="41">
-        <v>0</v>
-      </c>
-      <c r="S7" s="41">
-        <v>1</v>
-      </c>
-      <c r="T7" s="41">
-        <v>0</v>
-      </c>
-      <c r="U7" s="41">
-        <v>0</v>
-      </c>
-      <c r="V7" s="41">
-        <v>0</v>
-      </c>
-      <c r="W7" s="41">
-        <v>0</v>
-      </c>
-      <c r="X7" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="41">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="41">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="41">
-        <v>1</v>
-      </c>
-      <c r="AB7" s="41">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="40">
+      <c r="O7" s="42">
+        <v>0</v>
+      </c>
+      <c r="P7" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="42">
+        <v>0</v>
+      </c>
+      <c r="R7" s="42">
+        <v>0</v>
+      </c>
+      <c r="S7" s="42">
+        <v>0</v>
+      </c>
+      <c r="T7" s="42">
+        <v>1</v>
+      </c>
+      <c r="U7" s="42">
+        <v>0</v>
+      </c>
+      <c r="V7" s="42">
+        <v>0</v>
+      </c>
+      <c r="W7" s="42">
+        <v>0</v>
+      </c>
+      <c r="X7" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="42">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="42">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="42">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="42">
         <v>0</v>
       </c>
       <c r="AD7" s="41">
         <v>0</v>
       </c>
-      <c r="AE7" s="41">
+      <c r="AE7" s="42">
         <v>0</v>
       </c>
       <c r="AF7" s="42">
-        <v>1</v>
-      </c>
-      <c r="AG7" s="22" t="str">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="43">
+        <v>1</v>
+      </c>
+      <c r="AH7" s="22" t="str">
         <f t="shared" si="0"/>
         <v>0000001000</v>
       </c>
-      <c r="AH7" s="22" t="str">
+      <c r="AI7" s="22" t="str">
         <f t="shared" si="1"/>
         <v>0000100001</v>
       </c>
-      <c r="AI7" s="22" t="str">
+      <c r="AJ7" s="22" t="str">
         <f t="shared" si="2"/>
         <v>00000010000000100001</v>
       </c>
-      <c r="AJ7" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>***00100011</v>
-      </c>
-      <c r="AL7" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL7" ca="1">MY_BIN2HEX(AI7)</f>
+      <c r="AK7" s="23" t="str">
+        <f>_xlfn.CONCAT(B7:M7)</f>
+        <v>***000100011</v>
+      </c>
+      <c r="AM7" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM7" ca="1">MY_BIN2HEX(AJ7)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="8" spans="1:57" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:58" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>64</v>
       </c>
@@ -2006,37 +2042,37 @@
       <c r="C8" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E8" s="10">
         <v>0</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="28">
         <v>0</v>
       </c>
       <c r="G8" s="11">
-        <v>1</v>
-      </c>
-      <c r="H8" s="28">
-        <v>1</v>
-      </c>
-      <c r="I8" s="13">
-        <v>0</v>
-      </c>
-      <c r="J8" s="29">
-        <v>0</v>
-      </c>
-      <c r="K8" s="14">
-        <v>1</v>
-      </c>
-      <c r="L8" s="15">
-        <v>0</v>
-      </c>
-      <c r="M8" s="16">
-        <v>0</v>
-      </c>
-      <c r="N8" s="17">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>1</v>
+      </c>
+      <c r="I8" s="29">
+        <v>1</v>
+      </c>
+      <c r="J8" s="13">
+        <v>0</v>
+      </c>
+      <c r="K8" s="30">
+        <v>0</v>
+      </c>
+      <c r="L8" s="14">
+        <v>1</v>
+      </c>
+      <c r="M8" s="15">
+        <v>0</v>
+      </c>
+      <c r="N8" s="16">
         <v>0</v>
       </c>
       <c r="O8" s="17">
@@ -2067,13 +2103,13 @@
         <v>0</v>
       </c>
       <c r="X8" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y8" s="17">
         <v>1</v>
       </c>
       <c r="Z8" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA8" s="17">
         <v>0</v>
@@ -2090,149 +2126,155 @@
       <c r="AE8" s="17">
         <v>0</v>
       </c>
-      <c r="AF8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="22" t="str">
+      <c r="AF8" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="22" t="str">
         <f t="shared" si="0"/>
         <v>0000000000</v>
       </c>
-      <c r="AH8" s="22" t="str">
+      <c r="AI8" s="22" t="str">
         <f t="shared" si="1"/>
         <v>0110000000</v>
       </c>
-      <c r="AI8" s="22" t="str">
+      <c r="AJ8" s="22" t="str">
         <f t="shared" si="2"/>
         <v>00000000000110000000</v>
       </c>
-      <c r="AJ8" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>***00110010</v>
-      </c>
-      <c r="AL8" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL8" ca="1">MY_BIN2HEX(AI8)</f>
+      <c r="AK8" s="23" t="str">
+        <f>_xlfn.CONCAT(B8:M8)</f>
+        <v>***000110010</v>
+      </c>
+      <c r="AM8" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM8" ca="1">MY_BIN2HEX(AJ8)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="9" spans="1:57" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:58" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="33">
-        <v>0</v>
-      </c>
-      <c r="F9" s="34">
-        <v>0</v>
-      </c>
-      <c r="G9" s="34">
-        <v>1</v>
+      <c r="B9" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="34">
+        <v>0</v>
+      </c>
+      <c r="F9" s="44">
+        <v>0</v>
+      </c>
+      <c r="G9" s="35">
+        <v>0</v>
       </c>
       <c r="H9" s="35">
         <v>1</v>
       </c>
       <c r="I9" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="37">
         <v>0</v>
       </c>
       <c r="K9" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" s="39">
         <v>1</v>
       </c>
       <c r="M9" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9" s="41">
         <v>0</v>
       </c>
-      <c r="O9" s="41">
-        <v>0</v>
-      </c>
-      <c r="P9" s="41">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="41">
-        <v>0</v>
-      </c>
-      <c r="R9" s="41">
-        <v>0</v>
-      </c>
-      <c r="S9" s="41">
-        <v>0</v>
-      </c>
-      <c r="T9" s="41">
-        <v>0</v>
-      </c>
-      <c r="U9" s="41">
-        <v>1</v>
-      </c>
-      <c r="V9" s="41">
-        <v>0</v>
-      </c>
-      <c r="W9" s="41">
-        <v>0</v>
-      </c>
-      <c r="X9" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="41">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="41">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="41">
-        <v>1</v>
-      </c>
-      <c r="AB9" s="41">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="40">
+      <c r="O9" s="42">
+        <v>0</v>
+      </c>
+      <c r="P9" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="42">
+        <v>0</v>
+      </c>
+      <c r="R9" s="42">
+        <v>0</v>
+      </c>
+      <c r="S9" s="42">
+        <v>0</v>
+      </c>
+      <c r="T9" s="42">
+        <v>0</v>
+      </c>
+      <c r="U9" s="42">
+        <v>0</v>
+      </c>
+      <c r="V9" s="42">
+        <v>1</v>
+      </c>
+      <c r="W9" s="42">
+        <v>0</v>
+      </c>
+      <c r="X9" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="42">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="42">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="42">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="42">
         <v>0</v>
       </c>
       <c r="AD9" s="41">
         <v>0</v>
       </c>
-      <c r="AE9" s="41">
+      <c r="AE9" s="42">
         <v>0</v>
       </c>
       <c r="AF9" s="42">
-        <v>1</v>
-      </c>
-      <c r="AG9" s="22" t="str">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="43">
+        <v>1</v>
+      </c>
+      <c r="AH9" s="22" t="str">
         <f t="shared" si="0"/>
         <v>0000000010</v>
       </c>
-      <c r="AH9" s="22" t="str">
+      <c r="AI9" s="22" t="str">
         <f t="shared" si="1"/>
         <v>0000100001</v>
       </c>
-      <c r="AI9" s="22" t="str">
+      <c r="AJ9" s="22" t="str">
         <f t="shared" si="2"/>
         <v>00000000100000100001</v>
       </c>
-      <c r="AJ9" s="23" t="str">
-        <f>_xlfn.CONCAT(B9:L9)</f>
-        <v>***00110011</v>
-      </c>
-      <c r="AL9" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL9" ca="1">MY_BIN2HEX(AI9)</f>
+      <c r="AK9" s="23" t="str">
+        <f>_xlfn.CONCAT(B9:M9)</f>
+        <v>***000110011</v>
+      </c>
+      <c r="AM9" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM9" ca="1">MY_BIN2HEX(AJ9)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="10" spans="1:57" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:58" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>66</v>
       </c>
@@ -2242,37 +2284,37 @@
       <c r="C10" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E10" s="10">
         <v>0</v>
       </c>
-      <c r="F10" s="11">
-        <v>1</v>
+      <c r="F10" s="28">
+        <v>0</v>
       </c>
       <c r="G10" s="11">
-        <v>0</v>
-      </c>
-      <c r="H10" s="28">
-        <v>0</v>
-      </c>
-      <c r="I10" s="13">
-        <v>0</v>
-      </c>
-      <c r="J10" s="29">
-        <v>0</v>
-      </c>
-      <c r="K10" s="14">
-        <v>1</v>
-      </c>
-      <c r="L10" s="15">
-        <v>0</v>
-      </c>
-      <c r="M10" s="16">
-        <v>0</v>
-      </c>
-      <c r="N10" s="17">
+        <v>1</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0</v>
+      </c>
+      <c r="I10" s="29">
+        <v>0</v>
+      </c>
+      <c r="J10" s="13">
+        <v>0</v>
+      </c>
+      <c r="K10" s="30">
+        <v>0</v>
+      </c>
+      <c r="L10" s="14">
+        <v>1</v>
+      </c>
+      <c r="M10" s="15">
+        <v>0</v>
+      </c>
+      <c r="N10" s="16">
         <v>0</v>
       </c>
       <c r="O10" s="17">
@@ -2282,10 +2324,10 @@
         <v>0</v>
       </c>
       <c r="Q10" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R10" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10" s="17">
         <v>0</v>
@@ -2303,10 +2345,10 @@
         <v>0</v>
       </c>
       <c r="X10" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z10" s="17">
         <v>0</v>
@@ -2326,27 +2368,30 @@
       <c r="AE10" s="17">
         <v>0</v>
       </c>
-      <c r="AF10" s="18">
-        <v>1</v>
-      </c>
-      <c r="AG10" s="22" t="str">
+      <c r="AF10" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="18">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="22" t="str">
         <f t="shared" si="0"/>
         <v>0000100000</v>
       </c>
-      <c r="AH10" s="22" t="str">
+      <c r="AI10" s="22" t="str">
         <f t="shared" si="1"/>
         <v>0100000001</v>
       </c>
-      <c r="AI10" s="22" t="str">
+      <c r="AJ10" s="22" t="str">
         <f t="shared" si="2"/>
         <v>00001000000100000001</v>
       </c>
-      <c r="AL10" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL10" ca="1">MY_BIN2HEX(AI10)</f>
+      <c r="AM10" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM10" ca="1">MY_BIN2HEX(AJ10)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="11" spans="1:57" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:58" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>67</v>
       </c>
@@ -2356,37 +2401,37 @@
       <c r="C11" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E11" s="10">
         <v>0</v>
       </c>
-      <c r="F11" s="11">
-        <v>1</v>
+      <c r="F11" s="28">
+        <v>0</v>
       </c>
       <c r="G11" s="11">
-        <v>0</v>
-      </c>
-      <c r="H11" s="28">
-        <v>1</v>
-      </c>
-      <c r="I11" s="13">
-        <v>0</v>
-      </c>
-      <c r="J11" s="29">
-        <v>0</v>
-      </c>
-      <c r="K11" s="14">
-        <v>1</v>
-      </c>
-      <c r="L11" s="15">
-        <v>0</v>
-      </c>
-      <c r="M11" s="16">
-        <v>0</v>
-      </c>
-      <c r="N11" s="17">
+        <v>1</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="29">
+        <v>1</v>
+      </c>
+      <c r="J11" s="13">
+        <v>0</v>
+      </c>
+      <c r="K11" s="30">
+        <v>0</v>
+      </c>
+      <c r="L11" s="14">
+        <v>1</v>
+      </c>
+      <c r="M11" s="15">
+        <v>0</v>
+      </c>
+      <c r="N11" s="16">
         <v>0</v>
       </c>
       <c r="O11" s="17">
@@ -2402,10 +2447,10 @@
         <v>0</v>
       </c>
       <c r="S11" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T11" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11" s="17">
         <v>0</v>
@@ -2417,10 +2462,10 @@
         <v>0</v>
       </c>
       <c r="X11" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y11" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z11" s="17">
         <v>0</v>
@@ -2440,27 +2485,30 @@
       <c r="AE11" s="17">
         <v>0</v>
       </c>
-      <c r="AF11" s="18">
-        <v>1</v>
-      </c>
-      <c r="AG11" s="22" t="str">
+      <c r="AF11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="18">
+        <v>1</v>
+      </c>
+      <c r="AH11" s="22" t="str">
         <f t="shared" si="0"/>
         <v>0000001000</v>
       </c>
-      <c r="AH11" s="22" t="str">
+      <c r="AI11" s="22" t="str">
         <f t="shared" si="1"/>
         <v>0100000001</v>
       </c>
-      <c r="AI11" s="22" t="str">
+      <c r="AJ11" s="22" t="str">
         <f t="shared" si="2"/>
         <v>00000010000100000001</v>
       </c>
-      <c r="AL11" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL11" ca="1">MY_BIN2HEX(AI11)</f>
+      <c r="AM11" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM11" ca="1">MY_BIN2HEX(AJ11)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="12" spans="1:57" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:58" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>68</v>
       </c>
@@ -2470,37 +2518,37 @@
       <c r="C12" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E12" s="10">
         <v>0</v>
       </c>
-      <c r="F12" s="11">
-        <v>1</v>
+      <c r="F12" s="28">
+        <v>0</v>
       </c>
       <c r="G12" s="11">
         <v>1</v>
       </c>
-      <c r="H12" s="28">
-        <v>0</v>
-      </c>
-      <c r="I12" s="13">
-        <v>0</v>
-      </c>
-      <c r="J12" s="29">
-        <v>0</v>
-      </c>
-      <c r="K12" s="14">
-        <v>1</v>
-      </c>
-      <c r="L12" s="15">
-        <v>0</v>
-      </c>
-      <c r="M12" s="16">
-        <v>0</v>
-      </c>
-      <c r="N12" s="17">
+      <c r="H12" s="11">
+        <v>1</v>
+      </c>
+      <c r="I12" s="29">
+        <v>0</v>
+      </c>
+      <c r="J12" s="13">
+        <v>0</v>
+      </c>
+      <c r="K12" s="30">
+        <v>0</v>
+      </c>
+      <c r="L12" s="14">
+        <v>1</v>
+      </c>
+      <c r="M12" s="15">
+        <v>0</v>
+      </c>
+      <c r="N12" s="16">
         <v>0</v>
       </c>
       <c r="O12" s="17">
@@ -2522,19 +2570,19 @@
         <v>0</v>
       </c>
       <c r="U12" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V12" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W12" s="17">
         <v>0</v>
       </c>
       <c r="X12" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y12" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z12" s="17">
         <v>0</v>
@@ -2554,27 +2602,30 @@
       <c r="AE12" s="17">
         <v>0</v>
       </c>
-      <c r="AF12" s="18">
-        <v>1</v>
-      </c>
-      <c r="AG12" s="22" t="str">
+      <c r="AF12" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="18">
+        <v>1</v>
+      </c>
+      <c r="AH12" s="22" t="str">
         <f t="shared" si="0"/>
         <v>0000000010</v>
       </c>
-      <c r="AH12" s="22" t="str">
+      <c r="AI12" s="22" t="str">
         <f t="shared" si="1"/>
         <v>0100000001</v>
       </c>
-      <c r="AI12" s="22" t="str">
+      <c r="AJ12" s="22" t="str">
         <f t="shared" si="2"/>
         <v>00000000100100000001</v>
       </c>
-      <c r="AL12" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL12" ca="1">MY_BIN2HEX(AI12)</f>
+      <c r="AM12" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM12" ca="1">MY_BIN2HEX(AJ12)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="13" spans="1:57" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:58" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>69</v>
       </c>
@@ -2584,37 +2635,37 @@
       <c r="C13" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="10">
         <v>0</v>
       </c>
-      <c r="F13" s="11">
-        <v>1</v>
+      <c r="F13" s="28">
+        <v>0</v>
       </c>
       <c r="G13" s="11">
         <v>1</v>
       </c>
-      <c r="H13" s="28">
-        <v>1</v>
-      </c>
-      <c r="I13" s="13">
-        <v>0</v>
-      </c>
-      <c r="J13" s="29">
-        <v>0</v>
-      </c>
-      <c r="K13" s="14">
-        <v>1</v>
-      </c>
-      <c r="L13" s="15">
-        <v>0</v>
-      </c>
-      <c r="M13" s="16">
-        <v>0</v>
-      </c>
-      <c r="N13" s="17">
+      <c r="H13" s="11">
+        <v>1</v>
+      </c>
+      <c r="I13" s="29">
+        <v>1</v>
+      </c>
+      <c r="J13" s="13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="30">
+        <v>0</v>
+      </c>
+      <c r="L13" s="14">
+        <v>1</v>
+      </c>
+      <c r="M13" s="15">
+        <v>0</v>
+      </c>
+      <c r="N13" s="16">
         <v>0</v>
       </c>
       <c r="O13" s="17">
@@ -2645,13 +2696,13 @@
         <v>0</v>
       </c>
       <c r="X13" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y13" s="17">
         <v>1</v>
       </c>
       <c r="Z13" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA13" s="17">
         <v>0</v>
@@ -2668,27 +2719,30 @@
       <c r="AE13" s="17">
         <v>0</v>
       </c>
-      <c r="AF13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AG13" s="22" t="str">
-        <f t="shared" ref="AG13" si="5">_xlfn.CONCAT(M13:V13)</f>
+      <c r="AF13" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="22" t="str">
+        <f t="shared" ref="AH13" si="4">_xlfn.CONCAT(N13:W13)</f>
         <v>0000000000</v>
       </c>
-      <c r="AH13" s="22" t="str">
+      <c r="AI13" s="22" t="str">
         <f t="shared" si="1"/>
         <v>0110000000</v>
       </c>
-      <c r="AI13" s="22" t="str">
+      <c r="AJ13" s="22" t="str">
         <f t="shared" si="2"/>
         <v>00000000000110000000</v>
       </c>
-      <c r="AL13" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL13" ca="1">MY_BIN2HEX(AI13)</f>
+      <c r="AM13" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM13" ca="1">MY_BIN2HEX(AJ13)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="14" spans="1:57" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:58" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>70</v>
       </c>
@@ -2698,37 +2752,37 @@
       <c r="C14" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E14" s="10">
         <v>0</v>
       </c>
-      <c r="F14" s="11">
-        <v>1</v>
+      <c r="F14" s="28">
+        <v>0</v>
       </c>
       <c r="G14" s="11">
         <v>1</v>
       </c>
-      <c r="H14" s="28">
-        <v>1</v>
-      </c>
-      <c r="I14" s="13">
-        <v>0</v>
-      </c>
-      <c r="J14" s="29">
-        <v>0</v>
-      </c>
-      <c r="K14" s="14">
-        <v>1</v>
-      </c>
-      <c r="L14" s="15">
-        <v>1</v>
-      </c>
-      <c r="M14" s="16">
-        <v>0</v>
-      </c>
-      <c r="N14" s="17">
+      <c r="H14" s="11">
+        <v>1</v>
+      </c>
+      <c r="I14" s="29">
+        <v>1</v>
+      </c>
+      <c r="J14" s="13">
+        <v>0</v>
+      </c>
+      <c r="K14" s="30">
+        <v>0</v>
+      </c>
+      <c r="L14" s="14">
+        <v>1</v>
+      </c>
+      <c r="M14" s="15">
+        <v>1</v>
+      </c>
+      <c r="N14" s="16">
         <v>0</v>
       </c>
       <c r="O14" s="17">
@@ -2744,10 +2798,10 @@
         <v>0</v>
       </c>
       <c r="S14" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T14" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14" s="17">
         <v>0</v>
@@ -2768,10 +2822,10 @@
         <v>0</v>
       </c>
       <c r="AA14" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB14" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC14" s="17">
         <v>0</v>
@@ -2782,27 +2836,30 @@
       <c r="AE14" s="17">
         <v>0</v>
       </c>
-      <c r="AF14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AG14" s="22" t="str">
-        <f t="shared" ref="AG14" si="6">_xlfn.CONCAT(M14:V14)</f>
+      <c r="AF14" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="22" t="str">
+        <f t="shared" ref="AH14" si="5">_xlfn.CONCAT(N14:W14)</f>
         <v>0000001000</v>
       </c>
-      <c r="AH14" s="22" t="str">
+      <c r="AI14" s="22" t="str">
         <f t="shared" si="1"/>
         <v>0000100000</v>
       </c>
-      <c r="AI14" s="22" t="str">
+      <c r="AJ14" s="22" t="str">
         <f t="shared" si="2"/>
         <v>00000010000000100000</v>
       </c>
-      <c r="AL14" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL14" ca="1">MY_BIN2HEX(AI14)</f>
+      <c r="AM14" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM14" ca="1">MY_BIN2HEX(AJ14)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="15" spans="1:57" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:58" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>71</v>
       </c>
@@ -2812,37 +2869,37 @@
       <c r="C15" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E15" s="10">
         <v>0</v>
       </c>
-      <c r="F15" s="11">
-        <v>1</v>
+      <c r="F15" s="28">
+        <v>0</v>
       </c>
       <c r="G15" s="11">
         <v>1</v>
       </c>
-      <c r="H15" s="28">
-        <v>1</v>
-      </c>
-      <c r="I15" s="13">
-        <v>0</v>
-      </c>
-      <c r="J15" s="29">
-        <v>1</v>
-      </c>
-      <c r="K15" s="14">
-        <v>0</v>
-      </c>
-      <c r="L15" s="15">
-        <v>0</v>
-      </c>
-      <c r="M15" s="16">
-        <v>0</v>
-      </c>
-      <c r="N15" s="17">
+      <c r="H15" s="11">
+        <v>1</v>
+      </c>
+      <c r="I15" s="29">
+        <v>1</v>
+      </c>
+      <c r="J15" s="13">
+        <v>0</v>
+      </c>
+      <c r="K15" s="30">
+        <v>1</v>
+      </c>
+      <c r="L15" s="14">
+        <v>0</v>
+      </c>
+      <c r="M15" s="15">
+        <v>0</v>
+      </c>
+      <c r="N15" s="16">
         <v>0</v>
       </c>
       <c r="O15" s="17">
@@ -2864,10 +2921,10 @@
         <v>0</v>
       </c>
       <c r="U15" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V15" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W15" s="17">
         <v>0</v>
@@ -2885,38 +2942,41 @@
         <v>0</v>
       </c>
       <c r="AB15" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC15" s="17">
         <v>1</v>
       </c>
       <c r="AD15" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE15" s="17">
         <v>0</v>
       </c>
-      <c r="AF15" s="18">
-        <v>1</v>
-      </c>
-      <c r="AG15" s="22" t="str">
-        <f t="shared" ref="AG15" si="7">_xlfn.CONCAT(M15:V15)</f>
+      <c r="AF15" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="18">
+        <v>1</v>
+      </c>
+      <c r="AH15" s="22" t="str">
+        <f t="shared" ref="AH15" si="6">_xlfn.CONCAT(N15:W15)</f>
         <v>0000000010</v>
       </c>
-      <c r="AH15" s="22" t="str">
+      <c r="AI15" s="22" t="str">
         <f t="shared" si="1"/>
         <v>0000011001</v>
       </c>
-      <c r="AI15" s="22" t="str">
+      <c r="AJ15" s="22" t="str">
         <f t="shared" si="2"/>
         <v>00000000100000011001</v>
       </c>
-      <c r="AL15" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL15" ca="1">MY_BIN2HEX(AI15)</f>
+      <c r="AM15" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM15" ca="1">MY_BIN2HEX(AJ15)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="16" spans="1:57" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:58" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>72</v>
       </c>
@@ -2926,37 +2986,37 @@
       <c r="C16" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E16" s="10">
-        <v>1</v>
-      </c>
-      <c r="F16" s="11">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="F16" s="28">
+        <v>1</v>
       </c>
       <c r="G16" s="11">
         <v>0</v>
       </c>
-      <c r="H16" s="28">
-        <v>0</v>
-      </c>
-      <c r="I16" s="13">
-        <v>0</v>
-      </c>
-      <c r="J16" s="29">
-        <v>0</v>
-      </c>
-      <c r="K16" s="14">
-        <v>1</v>
-      </c>
-      <c r="L16" s="15">
-        <v>0</v>
-      </c>
-      <c r="M16" s="16">
-        <v>0</v>
-      </c>
-      <c r="N16" s="17">
+      <c r="H16" s="11">
+        <v>0</v>
+      </c>
+      <c r="I16" s="29">
+        <v>0</v>
+      </c>
+      <c r="J16" s="13">
+        <v>0</v>
+      </c>
+      <c r="K16" s="30">
+        <v>0</v>
+      </c>
+      <c r="L16" s="14">
+        <v>1</v>
+      </c>
+      <c r="M16" s="15">
+        <v>0</v>
+      </c>
+      <c r="N16" s="16">
         <v>0</v>
       </c>
       <c r="O16" s="17">
@@ -2987,13 +3047,13 @@
         <v>0</v>
       </c>
       <c r="X16" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y16" s="17">
         <v>1</v>
       </c>
       <c r="Z16" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA16" s="17">
         <v>0</v>
@@ -3010,27 +3070,30 @@
       <c r="AE16" s="17">
         <v>0</v>
       </c>
-      <c r="AF16" s="18">
-        <v>0</v>
-      </c>
-      <c r="AG16" s="22" t="str">
-        <f t="shared" ref="AG16" si="8">_xlfn.CONCAT(M16:V16)</f>
+      <c r="AF16" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="22" t="str">
+        <f t="shared" ref="AH16" si="7">_xlfn.CONCAT(N16:W16)</f>
         <v>0000000000</v>
       </c>
-      <c r="AH16" s="22" t="str">
-        <f t="shared" ref="AH16" si="9">_xlfn.CONCAT(W16:AF16)</f>
+      <c r="AI16" s="22" t="str">
+        <f t="shared" ref="AI16" si="8">_xlfn.CONCAT(X16:AG16)</f>
         <v>0110000000</v>
       </c>
-      <c r="AI16" s="22" t="str">
-        <f t="shared" ref="AI16" si="10">_xlfn.CONCAT(AG16:AH16)</f>
+      <c r="AJ16" s="22" t="str">
+        <f t="shared" ref="AJ16" si="9">_xlfn.CONCAT(AH16:AI16)</f>
         <v>00000000000110000000</v>
       </c>
-      <c r="AL16" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL16" ca="1">MY_BIN2HEX(AI16)</f>
+      <c r="AM16" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM16" ca="1">MY_BIN2HEX(AJ16)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="17" spans="1:38" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>73</v>
       </c>
@@ -3040,37 +3103,37 @@
       <c r="C17" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E17" s="10">
-        <v>1</v>
-      </c>
-      <c r="F17" s="11">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="F17" s="28">
+        <v>1</v>
       </c>
       <c r="G17" s="11">
         <v>0</v>
       </c>
-      <c r="H17" s="28">
-        <v>0</v>
-      </c>
-      <c r="I17" s="13">
-        <v>0</v>
-      </c>
-      <c r="J17" s="29">
-        <v>0</v>
-      </c>
-      <c r="K17" s="14">
-        <v>1</v>
-      </c>
-      <c r="L17" s="15">
-        <v>1</v>
-      </c>
-      <c r="M17" s="16">
-        <v>0</v>
-      </c>
-      <c r="N17" s="17">
+      <c r="H17" s="11">
+        <v>0</v>
+      </c>
+      <c r="I17" s="29">
+        <v>0</v>
+      </c>
+      <c r="J17" s="13">
+        <v>0</v>
+      </c>
+      <c r="K17" s="30">
+        <v>0</v>
+      </c>
+      <c r="L17" s="14">
+        <v>1</v>
+      </c>
+      <c r="M17" s="15">
+        <v>1</v>
+      </c>
+      <c r="N17" s="16">
         <v>0</v>
       </c>
       <c r="O17" s="17">
@@ -3086,10 +3149,10 @@
         <v>0</v>
       </c>
       <c r="S17" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T17" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U17" s="17">
         <v>0</v>
@@ -3110,10 +3173,10 @@
         <v>0</v>
       </c>
       <c r="AA17" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB17" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC17" s="17">
         <v>0</v>
@@ -3124,27 +3187,30 @@
       <c r="AE17" s="17">
         <v>0</v>
       </c>
-      <c r="AF17" s="18">
-        <v>0</v>
-      </c>
-      <c r="AG17" s="22" t="str">
-        <f t="shared" ref="AG17:AG20" si="11">_xlfn.CONCAT(M17:V17)</f>
+      <c r="AF17" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="22" t="str">
+        <f t="shared" ref="AH17:AH20" si="10">_xlfn.CONCAT(N17:W17)</f>
         <v>0000001000</v>
       </c>
-      <c r="AH17" s="22" t="str">
-        <f t="shared" ref="AH17:AH20" si="12">_xlfn.CONCAT(W17:AF17)</f>
+      <c r="AI17" s="22" t="str">
+        <f t="shared" ref="AI17:AI20" si="11">_xlfn.CONCAT(X17:AG17)</f>
         <v>0000100000</v>
       </c>
-      <c r="AI17" s="22" t="str">
-        <f t="shared" ref="AI17:AI20" si="13">_xlfn.CONCAT(AG17:AH17)</f>
+      <c r="AJ17" s="22" t="str">
+        <f t="shared" ref="AJ17:AJ20" si="12">_xlfn.CONCAT(AH17:AI17)</f>
         <v>00000010000000100000</v>
       </c>
-      <c r="AL17" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL17" ca="1">MY_BIN2HEX(AI17)</f>
+      <c r="AM17" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM17" ca="1">MY_BIN2HEX(AJ17)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="18" spans="1:38" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>74</v>
       </c>
@@ -3154,37 +3220,37 @@
       <c r="C18" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E18" s="10">
-        <v>1</v>
-      </c>
-      <c r="F18" s="11">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="F18" s="28">
+        <v>1</v>
       </c>
       <c r="G18" s="11">
         <v>0</v>
       </c>
-      <c r="H18" s="28">
-        <v>0</v>
-      </c>
-      <c r="I18" s="13">
-        <v>0</v>
-      </c>
-      <c r="J18" s="29">
-        <v>1</v>
-      </c>
-      <c r="K18" s="14">
-        <v>0</v>
-      </c>
-      <c r="L18" s="15">
-        <v>0</v>
-      </c>
-      <c r="M18" s="16">
-        <v>0</v>
-      </c>
-      <c r="N18" s="17">
+      <c r="H18" s="11">
+        <v>0</v>
+      </c>
+      <c r="I18" s="29">
+        <v>0</v>
+      </c>
+      <c r="J18" s="13">
+        <v>0</v>
+      </c>
+      <c r="K18" s="30">
+        <v>1</v>
+      </c>
+      <c r="L18" s="14">
+        <v>0</v>
+      </c>
+      <c r="M18" s="15">
+        <v>0</v>
+      </c>
+      <c r="N18" s="16">
         <v>0</v>
       </c>
       <c r="O18" s="17">
@@ -3206,10 +3272,10 @@
         <v>0</v>
       </c>
       <c r="U18" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V18" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W18" s="17">
         <v>0</v>
@@ -3227,7 +3293,7 @@
         <v>0</v>
       </c>
       <c r="AB18" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC18" s="17">
         <v>1</v>
@@ -3236,29 +3302,32 @@
         <v>1</v>
       </c>
       <c r="AE18" s="17">
-        <v>0</v>
-      </c>
-      <c r="AF18" s="18">
-        <v>1</v>
-      </c>
-      <c r="AG18" s="22" t="str">
+        <v>1</v>
+      </c>
+      <c r="AF18" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="18">
+        <v>1</v>
+      </c>
+      <c r="AH18" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>0000000010</v>
+      </c>
+      <c r="AI18" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>0000000010</v>
-      </c>
-      <c r="AH18" s="22" t="str">
+        <v>0000011101</v>
+      </c>
+      <c r="AJ18" s="22" t="str">
         <f t="shared" si="12"/>
-        <v>0000011101</v>
-      </c>
-      <c r="AI18" s="22" t="str">
-        <f t="shared" si="13"/>
         <v>00000000100000011101</v>
       </c>
-      <c r="AL18" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL18" ca="1">MY_BIN2HEX(AI18)</f>
+      <c r="AM18" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM18" ca="1">MY_BIN2HEX(AJ18)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="19" spans="1:38" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>75</v>
       </c>
@@ -3268,47 +3337,47 @@
       <c r="C19" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E19" s="10">
-        <v>1</v>
-      </c>
-      <c r="F19" s="11">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="F19" s="28">
+        <v>1</v>
       </c>
       <c r="G19" s="11">
         <v>0</v>
       </c>
-      <c r="H19" s="28">
-        <v>1</v>
-      </c>
-      <c r="I19" s="13">
-        <v>0</v>
-      </c>
-      <c r="J19" s="29">
-        <v>0</v>
-      </c>
-      <c r="K19" s="14">
-        <v>1</v>
-      </c>
-      <c r="L19" s="15">
-        <v>0</v>
-      </c>
-      <c r="M19" s="16">
-        <v>0</v>
-      </c>
-      <c r="N19" s="17">
+      <c r="H19" s="11">
+        <v>0</v>
+      </c>
+      <c r="I19" s="29">
+        <v>1</v>
+      </c>
+      <c r="J19" s="13">
+        <v>0</v>
+      </c>
+      <c r="K19" s="30">
+        <v>0</v>
+      </c>
+      <c r="L19" s="14">
+        <v>1</v>
+      </c>
+      <c r="M19" s="15">
+        <v>0</v>
+      </c>
+      <c r="N19" s="16">
         <v>0</v>
       </c>
       <c r="O19" s="17">
         <v>0</v>
       </c>
       <c r="P19" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R19" s="17">
         <v>0</v>
@@ -3329,10 +3398,10 @@
         <v>0</v>
       </c>
       <c r="X19" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y19" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z19" s="17">
         <v>0</v>
@@ -3352,27 +3421,30 @@
       <c r="AE19" s="17">
         <v>0</v>
       </c>
-      <c r="AF19" s="18">
-        <v>1</v>
-      </c>
-      <c r="AG19" s="22" t="str">
+      <c r="AF19" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="18">
+        <v>1</v>
+      </c>
+      <c r="AH19" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>0001000000</v>
+      </c>
+      <c r="AI19" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>0001000000</v>
-      </c>
-      <c r="AH19" s="22" t="str">
+        <v>0100000001</v>
+      </c>
+      <c r="AJ19" s="22" t="str">
         <f t="shared" si="12"/>
-        <v>0100000001</v>
-      </c>
-      <c r="AI19" s="22" t="str">
-        <f t="shared" si="13"/>
         <v>00010000000100000001</v>
       </c>
-      <c r="AL19" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL19" ca="1">MY_BIN2HEX(AI19)</f>
+      <c r="AM19" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM19" ca="1">MY_BIN2HEX(AJ19)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="20" spans="1:38" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:39" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>76</v>
       </c>
@@ -3382,37 +3454,37 @@
       <c r="C20" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E20" s="10">
-        <v>1</v>
-      </c>
-      <c r="F20" s="11">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="F20" s="28">
+        <v>1</v>
       </c>
       <c r="G20" s="11">
         <v>0</v>
       </c>
-      <c r="H20" s="28">
-        <v>1</v>
-      </c>
-      <c r="I20" s="13">
-        <v>0</v>
-      </c>
-      <c r="J20" s="29">
-        <v>0</v>
-      </c>
-      <c r="K20" s="14">
-        <v>1</v>
-      </c>
-      <c r="L20" s="15">
-        <v>0</v>
-      </c>
-      <c r="M20" s="16">
-        <v>0</v>
-      </c>
-      <c r="N20" s="17">
+      <c r="H20" s="11">
+        <v>1</v>
+      </c>
+      <c r="I20" s="29">
+        <v>0</v>
+      </c>
+      <c r="J20" s="13">
+        <v>0</v>
+      </c>
+      <c r="K20" s="30">
+        <v>0</v>
+      </c>
+      <c r="L20" s="14">
+        <v>1</v>
+      </c>
+      <c r="M20" s="15">
+        <v>0</v>
+      </c>
+      <c r="N20" s="16">
         <v>0</v>
       </c>
       <c r="O20" s="17">
@@ -3443,13 +3515,13 @@
         <v>0</v>
       </c>
       <c r="X20" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y20" s="17">
         <v>1</v>
       </c>
       <c r="Z20" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA20" s="17">
         <v>0</v>
@@ -3466,27 +3538,30 @@
       <c r="AE20" s="17">
         <v>0</v>
       </c>
-      <c r="AF20" s="18">
-        <v>0</v>
-      </c>
-      <c r="AG20" s="22" t="str">
+      <c r="AF20" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>0000000000</v>
+      </c>
+      <c r="AI20" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>0000000000</v>
-      </c>
-      <c r="AH20" s="22" t="str">
+        <v>0110000000</v>
+      </c>
+      <c r="AJ20" s="22" t="str">
         <f t="shared" si="12"/>
-        <v>0110000000</v>
-      </c>
-      <c r="AI20" s="22" t="str">
-        <f t="shared" si="13"/>
         <v>00000000000110000000</v>
       </c>
-      <c r="AL20" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL20" ca="1">MY_BIN2HEX(AI20)</f>
+      <c r="AM20" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM20" ca="1">MY_BIN2HEX(AJ20)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="21" spans="1:38" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:39" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>77</v>
       </c>
@@ -3496,37 +3571,37 @@
       <c r="C21" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E21" s="10">
-        <v>1</v>
-      </c>
-      <c r="F21" s="11">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="F21" s="28">
+        <v>1</v>
       </c>
       <c r="G21" s="11">
         <v>0</v>
       </c>
-      <c r="H21" s="28">
-        <v>1</v>
-      </c>
-      <c r="I21" s="13">
-        <v>0</v>
-      </c>
-      <c r="J21" s="29">
-        <v>0</v>
-      </c>
-      <c r="K21" s="14">
-        <v>1</v>
-      </c>
-      <c r="L21" s="15">
-        <v>1</v>
-      </c>
-      <c r="M21" s="16">
-        <v>0</v>
-      </c>
-      <c r="N21" s="17">
+      <c r="H21" s="11">
+        <v>1</v>
+      </c>
+      <c r="I21" s="29">
+        <v>0</v>
+      </c>
+      <c r="J21" s="13">
+        <v>0</v>
+      </c>
+      <c r="K21" s="30">
+        <v>0</v>
+      </c>
+      <c r="L21" s="14">
+        <v>1</v>
+      </c>
+      <c r="M21" s="15">
+        <v>1</v>
+      </c>
+      <c r="N21" s="16">
         <v>0</v>
       </c>
       <c r="O21" s="17">
@@ -3536,10 +3611,10 @@
         <v>0</v>
       </c>
       <c r="Q21" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R21" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S21" s="17">
         <v>0</v>
@@ -3569,38 +3644,41 @@
         <v>0</v>
       </c>
       <c r="AB21" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC21" s="17">
         <v>1</v>
       </c>
       <c r="AD21" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE21" s="17">
-        <v>1</v>
-      </c>
-      <c r="AF21" s="18">
-        <v>1</v>
-      </c>
-      <c r="AG21" s="22" t="str">
-        <f t="shared" ref="AG21:AG22" si="14">_xlfn.CONCAT(M21:V21)</f>
+        <v>0</v>
+      </c>
+      <c r="AF21" s="17">
+        <v>1</v>
+      </c>
+      <c r="AG21" s="18">
+        <v>1</v>
+      </c>
+      <c r="AH21" s="22" t="str">
+        <f t="shared" ref="AH21:AH22" si="13">_xlfn.CONCAT(N21:W21)</f>
         <v>0000100000</v>
       </c>
-      <c r="AH21" s="22" t="str">
-        <f t="shared" ref="AH21:AH22" si="15">_xlfn.CONCAT(W21:AF21)</f>
+      <c r="AI21" s="22" t="str">
+        <f t="shared" ref="AI21:AI22" si="14">_xlfn.CONCAT(X21:AG21)</f>
         <v>0000011011</v>
       </c>
-      <c r="AI21" s="22" t="str">
-        <f t="shared" ref="AI21:AI22" si="16">_xlfn.CONCAT(AG21:AH21)</f>
+      <c r="AJ21" s="22" t="str">
+        <f t="shared" ref="AJ21:AJ22" si="15">_xlfn.CONCAT(AH21:AI21)</f>
         <v>00001000000000011011</v>
       </c>
-      <c r="AL21" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL21" ca="1">MY_BIN2HEX(AI21)</f>
+      <c r="AM21" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM21" ca="1">MY_BIN2HEX(AJ21)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="22" spans="1:38" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:39" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>78</v>
       </c>
@@ -3610,37 +3688,37 @@
       <c r="C22" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E22" s="10">
-        <v>1</v>
-      </c>
-      <c r="F22" s="11">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="F22" s="28">
+        <v>1</v>
       </c>
       <c r="G22" s="11">
-        <v>1</v>
-      </c>
-      <c r="H22" s="28">
-        <v>0</v>
-      </c>
-      <c r="I22" s="13">
-        <v>0</v>
-      </c>
-      <c r="J22" s="29">
-        <v>0</v>
-      </c>
-      <c r="K22" s="14">
-        <v>1</v>
-      </c>
-      <c r="L22" s="15">
-        <v>0</v>
-      </c>
-      <c r="M22" s="16">
-        <v>0</v>
-      </c>
-      <c r="N22" s="17">
+        <v>0</v>
+      </c>
+      <c r="H22" s="11">
+        <v>1</v>
+      </c>
+      <c r="I22" s="29">
+        <v>1</v>
+      </c>
+      <c r="J22" s="13">
+        <v>0</v>
+      </c>
+      <c r="K22" s="30">
+        <v>0</v>
+      </c>
+      <c r="L22" s="14">
+        <v>1</v>
+      </c>
+      <c r="M22" s="15">
+        <v>0</v>
+      </c>
+      <c r="N22" s="16">
         <v>0</v>
       </c>
       <c r="O22" s="17">
@@ -3671,13 +3749,13 @@
         <v>0</v>
       </c>
       <c r="X22" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y22" s="17">
         <v>1</v>
       </c>
       <c r="Z22" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA22" s="17">
         <v>0</v>
@@ -3694,27 +3772,30 @@
       <c r="AE22" s="17">
         <v>0</v>
       </c>
-      <c r="AF22" s="18">
-        <v>0</v>
-      </c>
-      <c r="AG22" s="22" t="str">
+      <c r="AF22" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="22" t="str">
+        <f t="shared" si="13"/>
+        <v>0000000000</v>
+      </c>
+      <c r="AI22" s="22" t="str">
         <f t="shared" si="14"/>
-        <v>0000000000</v>
-      </c>
-      <c r="AH22" s="22" t="str">
+        <v>0110000000</v>
+      </c>
+      <c r="AJ22" s="22" t="str">
         <f t="shared" si="15"/>
-        <v>0110000000</v>
-      </c>
-      <c r="AI22" s="22" t="str">
-        <f t="shared" si="16"/>
         <v>00000000000110000000</v>
       </c>
-      <c r="AL22" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL22" ca="1">MY_BIN2HEX(AI22)</f>
+      <c r="AM22" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM22" ca="1">MY_BIN2HEX(AJ22)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="23" spans="1:38" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>79</v>
       </c>
@@ -3724,37 +3805,37 @@
       <c r="C23" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E23" s="10">
-        <v>1</v>
-      </c>
-      <c r="F23" s="11">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="F23" s="28">
+        <v>1</v>
       </c>
       <c r="G23" s="11">
-        <v>1</v>
-      </c>
-      <c r="H23" s="28">
-        <v>0</v>
-      </c>
-      <c r="I23" s="13">
-        <v>0</v>
-      </c>
-      <c r="J23" s="29">
-        <v>0</v>
-      </c>
-      <c r="K23" s="14">
-        <v>1</v>
-      </c>
-      <c r="L23" s="15">
-        <v>1</v>
-      </c>
-      <c r="M23" s="16">
-        <v>0</v>
-      </c>
-      <c r="N23" s="17">
+        <v>0</v>
+      </c>
+      <c r="H23" s="11">
+        <v>1</v>
+      </c>
+      <c r="I23" s="29">
+        <v>1</v>
+      </c>
+      <c r="J23" s="13">
+        <v>0</v>
+      </c>
+      <c r="K23" s="30">
+        <v>0</v>
+      </c>
+      <c r="L23" s="14">
+        <v>1</v>
+      </c>
+      <c r="M23" s="15">
+        <v>1</v>
+      </c>
+      <c r="N23" s="16">
         <v>0</v>
       </c>
       <c r="O23" s="17">
@@ -3770,10 +3851,10 @@
         <v>0</v>
       </c>
       <c r="S23" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T23" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U23" s="17">
         <v>0</v>
@@ -3797,35 +3878,240 @@
         <v>0</v>
       </c>
       <c r="AB23" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC23" s="17">
         <v>1</v>
       </c>
       <c r="AD23" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE23" s="17">
-        <v>1</v>
-      </c>
-      <c r="AF23" s="18">
-        <v>1</v>
-      </c>
-      <c r="AG23" s="22" t="str">
-        <f t="shared" ref="AG23" si="17">_xlfn.CONCAT(M23:V23)</f>
+        <v>0</v>
+      </c>
+      <c r="AF23" s="17">
+        <v>1</v>
+      </c>
+      <c r="AG23" s="18">
+        <v>1</v>
+      </c>
+      <c r="AH23" s="22" t="str">
+        <f t="shared" ref="AH23" si="16">_xlfn.CONCAT(N23:W23)</f>
         <v>0000001000</v>
       </c>
-      <c r="AH23" s="22" t="str">
-        <f t="shared" ref="AH23" si="18">_xlfn.CONCAT(W23:AF23)</f>
+      <c r="AI23" s="22" t="str">
+        <f t="shared" ref="AI23" si="17">_xlfn.CONCAT(X23:AG23)</f>
         <v>0000011011</v>
       </c>
-      <c r="AI23" s="22" t="str">
-        <f t="shared" ref="AI23" si="19">_xlfn.CONCAT(AG23:AH23)</f>
+      <c r="AJ23" s="22" t="str">
+        <f t="shared" ref="AJ23" si="18">_xlfn.CONCAT(AH23:AI23)</f>
         <v>00000010000000011011</v>
       </c>
-      <c r="AL23" s="22" t="e" cm="1">
-        <f t="array" aca="1" ref="AL23" ca="1">MY_BIN2HEX(AI23)</f>
+      <c r="AM23" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="AM23" ca="1">MY_BIN2HEX(AJ23)</f>
         <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="10">
+        <v>0</v>
+      </c>
+      <c r="F24" s="28">
+        <v>1</v>
+      </c>
+      <c r="G24" s="11">
+        <v>1</v>
+      </c>
+      <c r="H24" s="11">
+        <v>0</v>
+      </c>
+      <c r="I24" s="29">
+        <v>0</v>
+      </c>
+      <c r="J24" s="13">
+        <v>0</v>
+      </c>
+      <c r="K24" s="30">
+        <v>0</v>
+      </c>
+      <c r="L24" s="14">
+        <v>1</v>
+      </c>
+      <c r="M24" s="15">
+        <v>0</v>
+      </c>
+      <c r="N24" s="16">
+        <v>0</v>
+      </c>
+      <c r="O24" s="17">
+        <v>0</v>
+      </c>
+      <c r="P24" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="17">
+        <v>0</v>
+      </c>
+      <c r="R24" s="17">
+        <v>0</v>
+      </c>
+      <c r="S24" s="17">
+        <v>0</v>
+      </c>
+      <c r="T24" s="17">
+        <v>0</v>
+      </c>
+      <c r="U24" s="17">
+        <v>0</v>
+      </c>
+      <c r="V24" s="17">
+        <v>0</v>
+      </c>
+      <c r="W24" s="17">
+        <v>0</v>
+      </c>
+      <c r="X24" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA24" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE24" s="17">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG24" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="10">
+        <v>0</v>
+      </c>
+      <c r="F25" s="28">
+        <v>1</v>
+      </c>
+      <c r="G25" s="11">
+        <v>1</v>
+      </c>
+      <c r="H25" s="11">
+        <v>0</v>
+      </c>
+      <c r="I25" s="29">
+        <v>0</v>
+      </c>
+      <c r="J25" s="13">
+        <v>0</v>
+      </c>
+      <c r="K25" s="30">
+        <v>0</v>
+      </c>
+      <c r="L25" s="14">
+        <v>1</v>
+      </c>
+      <c r="M25" s="15">
+        <v>1</v>
+      </c>
+      <c r="N25" s="16">
+        <v>0</v>
+      </c>
+      <c r="O25" s="17">
+        <v>0</v>
+      </c>
+      <c r="P25" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="17">
+        <v>0</v>
+      </c>
+      <c r="R25" s="17">
+        <v>0</v>
+      </c>
+      <c r="S25" s="17">
+        <v>0</v>
+      </c>
+      <c r="T25" s="17">
+        <v>0</v>
+      </c>
+      <c r="U25" s="17">
+        <v>0</v>
+      </c>
+      <c r="V25" s="17">
+        <v>1</v>
+      </c>
+      <c r="W25" s="17">
+        <v>0</v>
+      </c>
+      <c r="X25" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="17">
+        <v>1</v>
+      </c>
+      <c r="AD25" s="17">
+        <v>1</v>
+      </c>
+      <c r="AE25" s="17">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="17">
+        <v>1</v>
+      </c>
+      <c r="AG25" s="18">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new jump if carry, jump if zero, jump is even instructions
</commit_message>
<xml_diff>
--- a/microcode/microcode.xlsx
+++ b/microcode/microcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faust\Documents\Programming\retro-cpu\microcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57294C6-7017-4E39-B562-C411D8C355B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BDA526-9C7D-477E-970D-8F72797D023C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="705" yWindow="3240" windowWidth="19950" windowHeight="13725" xr2:uid="{6E1463FF-F293-475C-B9F6-92700082F5EB}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="86">
   <si>
     <t>I0</t>
   </si>
@@ -305,13 +305,22 @@
   </si>
   <si>
     <t>INCZStep3</t>
+  </si>
+  <si>
+    <t>JMZStep2</t>
+  </si>
+  <si>
+    <t>JMCStep2</t>
+  </si>
+  <si>
+    <t>JMEStep2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,6 +353,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -577,7 +594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -703,6 +720,7 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,11 +1041,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15E04F54-319B-4A29-A4E0-3412CD7198C4}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:BF25"/>
+  <dimension ref="A1:BF37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,7 +1355,7 @@
         <v>00100000000010000000</v>
       </c>
       <c r="AK2" s="23" t="str">
-        <f>_xlfn.CONCAT(B2:M2)</f>
+        <f t="shared" ref="AK2:AK9" si="0">_xlfn.CONCAT(B2:M2)</f>
         <v>********0000</v>
       </c>
       <c r="AL2" s="23" t="e">
@@ -1504,23 +1522,23 @@
         <v>1</v>
       </c>
       <c r="AH3" s="22" t="str">
-        <f t="shared" ref="AH3:AH12" si="0">_xlfn.CONCAT(N3:W3)</f>
+        <f t="shared" ref="AH3:AH12" si="1">_xlfn.CONCAT(N3:W3)</f>
         <v>0100000000</v>
       </c>
       <c r="AI3" s="22" t="str">
-        <f t="shared" ref="AI3:AI15" si="1">_xlfn.CONCAT(X3:AG3)</f>
+        <f t="shared" ref="AI3:AI15" si="2">_xlfn.CONCAT(X3:AG3)</f>
         <v>1000100001</v>
       </c>
       <c r="AJ3" s="22" t="str">
-        <f t="shared" ref="AJ3:AJ15" si="2">_xlfn.CONCAT(AH3:AI3)</f>
+        <f t="shared" ref="AJ3:AJ15" si="3">_xlfn.CONCAT(AH3:AI3)</f>
         <v>01000000001000100001</v>
       </c>
       <c r="AK3" s="23" t="str">
-        <f>_xlfn.CONCAT(B3:M3)</f>
+        <f t="shared" si="0"/>
         <v>********0001</v>
       </c>
       <c r="AL3" s="23" t="e">
-        <f t="shared" ref="AL3:AL5" si="3">BIN2HEX(AK3,5)</f>
+        <f t="shared" ref="AL3:AL5" si="4">BIN2HEX(AK3,5)</f>
         <v>#NUM!</v>
       </c>
       <c r="AM3" s="22" t="e" cm="1">
@@ -1633,23 +1651,23 @@
         <v>0</v>
       </c>
       <c r="AH4" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v>0000000000</v>
+      </c>
+      <c r="AI4" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>0110000000</v>
+      </c>
+      <c r="AJ4" s="22" t="str">
+        <f t="shared" si="3"/>
+        <v>00000000000110000000</v>
+      </c>
+      <c r="AK4" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>0000000000</v>
-      </c>
-      <c r="AI4" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>0110000000</v>
-      </c>
-      <c r="AJ4" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>00000000000110000000</v>
-      </c>
-      <c r="AK4" s="23" t="str">
-        <f>_xlfn.CONCAT(B4:M4)</f>
         <v>***000010010</v>
       </c>
       <c r="AL4" s="23" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
       <c r="AM4" s="22" t="e" cm="1">
@@ -1762,23 +1780,23 @@
         <v>1</v>
       </c>
       <c r="AH5" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v>0000100000</v>
+      </c>
+      <c r="AI5" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>0000100001</v>
+      </c>
+      <c r="AJ5" s="22" t="str">
+        <f t="shared" si="3"/>
+        <v>00001000000000100001</v>
+      </c>
+      <c r="AK5" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>0000100000</v>
-      </c>
-      <c r="AI5" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>0000100001</v>
-      </c>
-      <c r="AJ5" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>00001000000000100001</v>
-      </c>
-      <c r="AK5" s="23" t="str">
-        <f>_xlfn.CONCAT(B5:M5)</f>
         <v>***000010011</v>
       </c>
       <c r="AL5" s="23" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
       <c r="AM5" s="22" t="e" cm="1">
@@ -1891,19 +1909,19 @@
         <v>0</v>
       </c>
       <c r="AH6" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v>0000000000</v>
+      </c>
+      <c r="AI6" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>0110000000</v>
+      </c>
+      <c r="AJ6" s="22" t="str">
+        <f t="shared" si="3"/>
+        <v>00000000000110000000</v>
+      </c>
+      <c r="AK6" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>0000000000</v>
-      </c>
-      <c r="AI6" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>0110000000</v>
-      </c>
-      <c r="AJ6" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>00000000000110000000</v>
-      </c>
-      <c r="AK6" s="23" t="str">
-        <f>_xlfn.CONCAT(B6:M6)</f>
         <v>***000100010</v>
       </c>
       <c r="AM6" s="22" t="e" cm="1">
@@ -2012,19 +2030,19 @@
         <v>1</v>
       </c>
       <c r="AH7" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v>0000001000</v>
+      </c>
+      <c r="AI7" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>0000100001</v>
+      </c>
+      <c r="AJ7" s="22" t="str">
+        <f t="shared" si="3"/>
+        <v>00000010000000100001</v>
+      </c>
+      <c r="AK7" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>0000001000</v>
-      </c>
-      <c r="AI7" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>0000100001</v>
-      </c>
-      <c r="AJ7" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>00000010000000100001</v>
-      </c>
-      <c r="AK7" s="23" t="str">
-        <f>_xlfn.CONCAT(B7:M7)</f>
         <v>***000100011</v>
       </c>
       <c r="AM7" s="22" t="e" cm="1">
@@ -2133,19 +2151,19 @@
         <v>0</v>
       </c>
       <c r="AH8" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v>0000000000</v>
+      </c>
+      <c r="AI8" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>0110000000</v>
+      </c>
+      <c r="AJ8" s="22" t="str">
+        <f t="shared" si="3"/>
+        <v>00000000000110000000</v>
+      </c>
+      <c r="AK8" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>0000000000</v>
-      </c>
-      <c r="AI8" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>0110000000</v>
-      </c>
-      <c r="AJ8" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>00000000000110000000</v>
-      </c>
-      <c r="AK8" s="23" t="str">
-        <f>_xlfn.CONCAT(B8:M8)</f>
         <v>***000110010</v>
       </c>
       <c r="AM8" s="22" t="e" cm="1">
@@ -2254,19 +2272,19 @@
         <v>1</v>
       </c>
       <c r="AH9" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v>0000000010</v>
+      </c>
+      <c r="AI9" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>0000100001</v>
+      </c>
+      <c r="AJ9" s="22" t="str">
+        <f t="shared" si="3"/>
+        <v>00000000100000100001</v>
+      </c>
+      <c r="AK9" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>0000000010</v>
-      </c>
-      <c r="AI9" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>0000100001</v>
-      </c>
-      <c r="AJ9" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>00000000100000100001</v>
-      </c>
-      <c r="AK9" s="23" t="str">
-        <f>_xlfn.CONCAT(B9:M9)</f>
         <v>***000110011</v>
       </c>
       <c r="AM9" s="22" t="e" cm="1">
@@ -2375,15 +2393,15 @@
         <v>1</v>
       </c>
       <c r="AH10" s="22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0000100000</v>
       </c>
       <c r="AI10" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0100000001</v>
       </c>
       <c r="AJ10" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00001000000100000001</v>
       </c>
       <c r="AM10" s="22" t="e" cm="1">
@@ -2492,15 +2510,15 @@
         <v>1</v>
       </c>
       <c r="AH11" s="22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0000001000</v>
       </c>
       <c r="AI11" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0100000001</v>
       </c>
       <c r="AJ11" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000010000100000001</v>
       </c>
       <c r="AM11" s="22" t="e" cm="1">
@@ -2609,15 +2627,15 @@
         <v>1</v>
       </c>
       <c r="AH12" s="22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0000000010</v>
       </c>
       <c r="AI12" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0100000001</v>
       </c>
       <c r="AJ12" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000000100100000001</v>
       </c>
       <c r="AM12" s="22" t="e" cm="1">
@@ -2726,15 +2744,15 @@
         <v>0</v>
       </c>
       <c r="AH13" s="22" t="str">
-        <f t="shared" ref="AH13" si="4">_xlfn.CONCAT(N13:W13)</f>
+        <f t="shared" ref="AH13" si="5">_xlfn.CONCAT(N13:W13)</f>
         <v>0000000000</v>
       </c>
       <c r="AI13" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0110000000</v>
       </c>
       <c r="AJ13" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000000000110000000</v>
       </c>
       <c r="AM13" s="22" t="e" cm="1">
@@ -2843,15 +2861,15 @@
         <v>0</v>
       </c>
       <c r="AH14" s="22" t="str">
-        <f t="shared" ref="AH14" si="5">_xlfn.CONCAT(N14:W14)</f>
+        <f t="shared" ref="AH14" si="6">_xlfn.CONCAT(N14:W14)</f>
         <v>0000001000</v>
       </c>
       <c r="AI14" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0000100000</v>
       </c>
       <c r="AJ14" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000010000000100000</v>
       </c>
       <c r="AM14" s="22" t="e" cm="1">
@@ -2960,15 +2978,15 @@
         <v>1</v>
       </c>
       <c r="AH15" s="22" t="str">
-        <f t="shared" ref="AH15" si="6">_xlfn.CONCAT(N15:W15)</f>
+        <f t="shared" ref="AH15" si="7">_xlfn.CONCAT(N15:W15)</f>
         <v>0000000010</v>
       </c>
       <c r="AI15" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0000011001</v>
       </c>
       <c r="AJ15" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000000100000011001</v>
       </c>
       <c r="AM15" s="22" t="e" cm="1">
@@ -3077,15 +3095,15 @@
         <v>0</v>
       </c>
       <c r="AH16" s="22" t="str">
-        <f t="shared" ref="AH16" si="7">_xlfn.CONCAT(N16:W16)</f>
+        <f t="shared" ref="AH16" si="8">_xlfn.CONCAT(N16:W16)</f>
         <v>0000000000</v>
       </c>
       <c r="AI16" s="22" t="str">
-        <f t="shared" ref="AI16" si="8">_xlfn.CONCAT(X16:AG16)</f>
+        <f t="shared" ref="AI16" si="9">_xlfn.CONCAT(X16:AG16)</f>
         <v>0110000000</v>
       </c>
       <c r="AJ16" s="22" t="str">
-        <f t="shared" ref="AJ16" si="9">_xlfn.CONCAT(AH16:AI16)</f>
+        <f t="shared" ref="AJ16" si="10">_xlfn.CONCAT(AH16:AI16)</f>
         <v>00000000000110000000</v>
       </c>
       <c r="AM16" s="22" t="e" cm="1">
@@ -3194,15 +3212,15 @@
         <v>0</v>
       </c>
       <c r="AH17" s="22" t="str">
-        <f t="shared" ref="AH17:AH20" si="10">_xlfn.CONCAT(N17:W17)</f>
+        <f t="shared" ref="AH17:AH20" si="11">_xlfn.CONCAT(N17:W17)</f>
         <v>0000001000</v>
       </c>
       <c r="AI17" s="22" t="str">
-        <f t="shared" ref="AI17:AI20" si="11">_xlfn.CONCAT(X17:AG17)</f>
+        <f t="shared" ref="AI17:AI20" si="12">_xlfn.CONCAT(X17:AG17)</f>
         <v>0000100000</v>
       </c>
       <c r="AJ17" s="22" t="str">
-        <f t="shared" ref="AJ17:AJ20" si="12">_xlfn.CONCAT(AH17:AI17)</f>
+        <f t="shared" ref="AJ17:AJ20" si="13">_xlfn.CONCAT(AH17:AI17)</f>
         <v>00000010000000100000</v>
       </c>
       <c r="AM17" s="22" t="e" cm="1">
@@ -3311,15 +3329,15 @@
         <v>1</v>
       </c>
       <c r="AH18" s="22" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0000000010</v>
       </c>
       <c r="AI18" s="22" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0000011101</v>
       </c>
       <c r="AJ18" s="22" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>00000000100000011101</v>
       </c>
       <c r="AM18" s="22" t="e" cm="1">
@@ -3428,15 +3446,15 @@
         <v>1</v>
       </c>
       <c r="AH19" s="22" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0001000000</v>
       </c>
       <c r="AI19" s="22" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0100000001</v>
       </c>
       <c r="AJ19" s="22" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>00010000000100000001</v>
       </c>
       <c r="AM19" s="22" t="e" cm="1">
@@ -3545,15 +3563,15 @@
         <v>0</v>
       </c>
       <c r="AH20" s="22" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0000000000</v>
       </c>
       <c r="AI20" s="22" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0110000000</v>
       </c>
       <c r="AJ20" s="22" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>00000000000110000000</v>
       </c>
       <c r="AM20" s="22" t="e" cm="1">
@@ -3662,15 +3680,15 @@
         <v>1</v>
       </c>
       <c r="AH21" s="22" t="str">
-        <f t="shared" ref="AH21:AH22" si="13">_xlfn.CONCAT(N21:W21)</f>
+        <f t="shared" ref="AH21:AH22" si="14">_xlfn.CONCAT(N21:W21)</f>
         <v>0000100000</v>
       </c>
       <c r="AI21" s="22" t="str">
-        <f t="shared" ref="AI21:AI22" si="14">_xlfn.CONCAT(X21:AG21)</f>
+        <f t="shared" ref="AI21:AI22" si="15">_xlfn.CONCAT(X21:AG21)</f>
         <v>0000011011</v>
       </c>
       <c r="AJ21" s="22" t="str">
-        <f t="shared" ref="AJ21:AJ22" si="15">_xlfn.CONCAT(AH21:AI21)</f>
+        <f t="shared" ref="AJ21:AJ22" si="16">_xlfn.CONCAT(AH21:AI21)</f>
         <v>00001000000000011011</v>
       </c>
       <c r="AM21" s="22" t="e" cm="1">
@@ -3779,15 +3797,15 @@
         <v>0</v>
       </c>
       <c r="AH22" s="22" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0000000000</v>
       </c>
       <c r="AI22" s="22" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0110000000</v>
       </c>
       <c r="AJ22" s="22" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>00000000000110000000</v>
       </c>
       <c r="AM22" s="22" t="e" cm="1">
@@ -3896,15 +3914,15 @@
         <v>1</v>
       </c>
       <c r="AH23" s="22" t="str">
-        <f t="shared" ref="AH23" si="16">_xlfn.CONCAT(N23:W23)</f>
+        <f t="shared" ref="AH23" si="17">_xlfn.CONCAT(N23:W23)</f>
         <v>0000001000</v>
       </c>
       <c r="AI23" s="22" t="str">
-        <f t="shared" ref="AI23" si="17">_xlfn.CONCAT(X23:AG23)</f>
+        <f t="shared" ref="AI23" si="18">_xlfn.CONCAT(X23:AG23)</f>
         <v>0000011011</v>
       </c>
       <c r="AJ23" s="22" t="str">
-        <f t="shared" ref="AJ23" si="18">_xlfn.CONCAT(AH23:AI23)</f>
+        <f t="shared" ref="AJ23" si="19">_xlfn.CONCAT(AH23:AI23)</f>
         <v>00000010000000011011</v>
       </c>
       <c r="AM23" s="22" t="e" cm="1">
@@ -4013,7 +4031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:39" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>82</v>
       </c>
@@ -4113,6 +4131,312 @@
       <c r="AG25" s="18">
         <v>1</v>
       </c>
+    </row>
+    <row r="26" spans="1:39" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="11">
+        <v>1</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="10">
+        <v>0</v>
+      </c>
+      <c r="F26" s="28">
+        <v>1</v>
+      </c>
+      <c r="G26" s="11">
+        <v>1</v>
+      </c>
+      <c r="H26" s="11">
+        <v>0</v>
+      </c>
+      <c r="I26" s="29">
+        <v>1</v>
+      </c>
+      <c r="J26" s="13">
+        <v>0</v>
+      </c>
+      <c r="K26" s="30">
+        <v>0</v>
+      </c>
+      <c r="L26" s="14">
+        <v>1</v>
+      </c>
+      <c r="M26" s="15">
+        <v>1</v>
+      </c>
+      <c r="N26" s="16">
+        <v>0</v>
+      </c>
+      <c r="O26" s="17">
+        <v>0</v>
+      </c>
+      <c r="P26" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="17">
+        <v>1</v>
+      </c>
+      <c r="R26" s="17">
+        <v>0</v>
+      </c>
+      <c r="S26" s="17">
+        <v>0</v>
+      </c>
+      <c r="T26" s="17">
+        <v>0</v>
+      </c>
+      <c r="U26" s="17">
+        <v>0</v>
+      </c>
+      <c r="V26" s="17">
+        <v>0</v>
+      </c>
+      <c r="W26" s="17">
+        <v>0</v>
+      </c>
+      <c r="X26" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG26" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="29">
+        <v>1</v>
+      </c>
+      <c r="E27" s="10">
+        <v>0</v>
+      </c>
+      <c r="F27" s="28">
+        <v>1</v>
+      </c>
+      <c r="G27" s="11">
+        <v>1</v>
+      </c>
+      <c r="H27" s="11">
+        <v>1</v>
+      </c>
+      <c r="I27" s="29">
+        <v>0</v>
+      </c>
+      <c r="J27" s="13">
+        <v>0</v>
+      </c>
+      <c r="K27" s="30">
+        <v>0</v>
+      </c>
+      <c r="L27" s="14">
+        <v>1</v>
+      </c>
+      <c r="M27" s="15">
+        <v>1</v>
+      </c>
+      <c r="N27" s="16">
+        <v>0</v>
+      </c>
+      <c r="O27" s="17">
+        <v>0</v>
+      </c>
+      <c r="P27" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="17">
+        <v>1</v>
+      </c>
+      <c r="R27" s="17">
+        <v>0</v>
+      </c>
+      <c r="S27" s="17">
+        <v>0</v>
+      </c>
+      <c r="T27" s="17">
+        <v>0</v>
+      </c>
+      <c r="U27" s="17">
+        <v>0</v>
+      </c>
+      <c r="V27" s="17">
+        <v>0</v>
+      </c>
+      <c r="W27" s="17">
+        <v>0</v>
+      </c>
+      <c r="X27" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="17">
+        <v>0</v>
+      </c>
+      <c r="AF27" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG27" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="10">
+        <v>1</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="10">
+        <v>0</v>
+      </c>
+      <c r="F28" s="28">
+        <v>1</v>
+      </c>
+      <c r="G28" s="11">
+        <v>1</v>
+      </c>
+      <c r="H28" s="11">
+        <v>1</v>
+      </c>
+      <c r="I28" s="29">
+        <v>1</v>
+      </c>
+      <c r="J28" s="13">
+        <v>0</v>
+      </c>
+      <c r="K28" s="30">
+        <v>0</v>
+      </c>
+      <c r="L28" s="14">
+        <v>1</v>
+      </c>
+      <c r="M28" s="15">
+        <v>1</v>
+      </c>
+      <c r="N28" s="16">
+        <v>0</v>
+      </c>
+      <c r="O28" s="17">
+        <v>0</v>
+      </c>
+      <c r="P28" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="17">
+        <v>1</v>
+      </c>
+      <c r="R28" s="17">
+        <v>0</v>
+      </c>
+      <c r="S28" s="17">
+        <v>0</v>
+      </c>
+      <c r="T28" s="17">
+        <v>0</v>
+      </c>
+      <c r="U28" s="17">
+        <v>0</v>
+      </c>
+      <c r="V28" s="17">
+        <v>0</v>
+      </c>
+      <c r="W28" s="17">
+        <v>0</v>
+      </c>
+      <c r="X28" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="17">
+        <v>0</v>
+      </c>
+      <c r="AF28" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG28" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N37" s="45"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Improved cpu layout in logisim
</commit_message>
<xml_diff>
--- a/microcode/microcode.xlsx
+++ b/microcode/microcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faust\Documents\Programming\retro-cpu\microcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BDA526-9C7D-477E-970D-8F72797D023C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BAC2B6-040B-4AC5-A9EE-12CC225DD187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="705" yWindow="3240" windowWidth="19950" windowHeight="13725" xr2:uid="{6E1463FF-F293-475C-B9F6-92700082F5EB}"/>
   </bookViews>
@@ -1045,7 +1045,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I29" sqref="I29"/>
+      <selection pane="bottomLeft" activeCell="AK37" sqref="AK37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,7 +1057,7 @@
     <col min="34" max="34" width="16.140625" customWidth="1"/>
     <col min="35" max="35" width="15.85546875" customWidth="1"/>
     <col min="36" max="36" width="28.140625" customWidth="1"/>
-    <col min="37" max="37" width="14" customWidth="1"/>
+    <col min="37" max="37" width="17.42578125" customWidth="1"/>
     <col min="38" max="38" width="16.7109375" customWidth="1"/>
     <col min="39" max="39" width="19" customWidth="1"/>
     <col min="41" max="41" width="31.140625" customWidth="1"/>
@@ -1355,7 +1355,7 @@
         <v>00100000000010000000</v>
       </c>
       <c r="AK2" s="23" t="str">
-        <f t="shared" ref="AK2:AK9" si="0">_xlfn.CONCAT(B2:M2)</f>
+        <f t="shared" ref="AK2:AK28" si="0">_xlfn.CONCAT(B2:M2)</f>
         <v>********0000</v>
       </c>
       <c r="AL2" s="23" t="e">
@@ -2404,6 +2404,10 @@
         <f t="shared" si="3"/>
         <v>00001000000100000001</v>
       </c>
+      <c r="AK10" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>***001000010</v>
+      </c>
       <c r="AM10" s="22" t="e" cm="1">
         <f t="array" aca="1" ref="AM10" ca="1">MY_BIN2HEX(AJ10)</f>
         <v>#NAME?</v>
@@ -2521,6 +2525,10 @@
         <f t="shared" si="3"/>
         <v>00000010000100000001</v>
       </c>
+      <c r="AK11" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>***001010010</v>
+      </c>
       <c r="AM11" s="22" t="e" cm="1">
         <f t="array" aca="1" ref="AM11" ca="1">MY_BIN2HEX(AJ11)</f>
         <v>#NAME?</v>
@@ -2638,6 +2646,10 @@
         <f t="shared" si="3"/>
         <v>00000000100100000001</v>
       </c>
+      <c r="AK12" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>***001100010</v>
+      </c>
       <c r="AM12" s="22" t="e" cm="1">
         <f t="array" aca="1" ref="AM12" ca="1">MY_BIN2HEX(AJ12)</f>
         <v>#NAME?</v>
@@ -2755,6 +2767,10 @@
         <f t="shared" si="3"/>
         <v>00000000000110000000</v>
       </c>
+      <c r="AK13" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>***001110010</v>
+      </c>
       <c r="AM13" s="22" t="e" cm="1">
         <f t="array" aca="1" ref="AM13" ca="1">MY_BIN2HEX(AJ13)</f>
         <v>#NAME?</v>
@@ -2872,6 +2888,10 @@
         <f t="shared" si="3"/>
         <v>00000010000000100000</v>
       </c>
+      <c r="AK14" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>***001110011</v>
+      </c>
       <c r="AM14" s="22" t="e" cm="1">
         <f t="array" aca="1" ref="AM14" ca="1">MY_BIN2HEX(AJ14)</f>
         <v>#NAME?</v>
@@ -2989,6 +3009,10 @@
         <f t="shared" si="3"/>
         <v>00000000100000011001</v>
       </c>
+      <c r="AK15" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>***001110100</v>
+      </c>
       <c r="AM15" s="22" t="e" cm="1">
         <f t="array" aca="1" ref="AM15" ca="1">MY_BIN2HEX(AJ15)</f>
         <v>#NAME?</v>
@@ -3106,6 +3130,10 @@
         <f t="shared" ref="AJ16" si="10">_xlfn.CONCAT(AH16:AI16)</f>
         <v>00000000000110000000</v>
       </c>
+      <c r="AK16" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>***010000010</v>
+      </c>
       <c r="AM16" s="22" t="e" cm="1">
         <f t="array" aca="1" ref="AM16" ca="1">MY_BIN2HEX(AJ16)</f>
         <v>#NAME?</v>
@@ -3223,6 +3251,10 @@
         <f t="shared" ref="AJ17:AJ20" si="13">_xlfn.CONCAT(AH17:AI17)</f>
         <v>00000010000000100000</v>
       </c>
+      <c r="AK17" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>***010000011</v>
+      </c>
       <c r="AM17" s="22" t="e" cm="1">
         <f t="array" aca="1" ref="AM17" ca="1">MY_BIN2HEX(AJ17)</f>
         <v>#NAME?</v>
@@ -3340,6 +3372,10 @@
         <f t="shared" si="13"/>
         <v>00000000100000011101</v>
       </c>
+      <c r="AK18" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>***010000100</v>
+      </c>
       <c r="AM18" s="22" t="e" cm="1">
         <f t="array" aca="1" ref="AM18" ca="1">MY_BIN2HEX(AJ18)</f>
         <v>#NAME?</v>
@@ -3457,6 +3493,10 @@
         <f t="shared" si="13"/>
         <v>00010000000100000001</v>
       </c>
+      <c r="AK19" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>***010010010</v>
+      </c>
       <c r="AM19" s="22" t="e" cm="1">
         <f t="array" aca="1" ref="AM19" ca="1">MY_BIN2HEX(AJ19)</f>
         <v>#NAME?</v>
@@ -3574,6 +3614,10 @@
         <f t="shared" si="13"/>
         <v>00000000000110000000</v>
       </c>
+      <c r="AK20" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>***010100010</v>
+      </c>
       <c r="AM20" s="22" t="e" cm="1">
         <f t="array" aca="1" ref="AM20" ca="1">MY_BIN2HEX(AJ20)</f>
         <v>#NAME?</v>
@@ -3691,6 +3735,10 @@
         <f t="shared" ref="AJ21:AJ22" si="16">_xlfn.CONCAT(AH21:AI21)</f>
         <v>00001000000000011011</v>
       </c>
+      <c r="AK21" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>***010100011</v>
+      </c>
       <c r="AM21" s="22" t="e" cm="1">
         <f t="array" aca="1" ref="AM21" ca="1">MY_BIN2HEX(AJ21)</f>
         <v>#NAME?</v>
@@ -3808,6 +3856,10 @@
         <f t="shared" si="16"/>
         <v>00000000000110000000</v>
       </c>
+      <c r="AK22" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>***010110010</v>
+      </c>
       <c r="AM22" s="22" t="e" cm="1">
         <f t="array" aca="1" ref="AM22" ca="1">MY_BIN2HEX(AJ22)</f>
         <v>#NAME?</v>
@@ -3914,16 +3966,20 @@
         <v>1</v>
       </c>
       <c r="AH23" s="22" t="str">
-        <f t="shared" ref="AH23" si="17">_xlfn.CONCAT(N23:W23)</f>
+        <f t="shared" ref="AH23:AH28" si="17">_xlfn.CONCAT(N23:W23)</f>
         <v>0000001000</v>
       </c>
       <c r="AI23" s="22" t="str">
-        <f t="shared" ref="AI23" si="18">_xlfn.CONCAT(X23:AG23)</f>
+        <f t="shared" ref="AI23:AI28" si="18">_xlfn.CONCAT(X23:AG23)</f>
         <v>0000011011</v>
       </c>
       <c r="AJ23" s="22" t="str">
-        <f t="shared" ref="AJ23" si="19">_xlfn.CONCAT(AH23:AI23)</f>
+        <f t="shared" ref="AJ23:AJ28" si="19">_xlfn.CONCAT(AH23:AI23)</f>
         <v>00000010000000011011</v>
+      </c>
+      <c r="AK23" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>***010110011</v>
       </c>
       <c r="AM23" s="22" t="e" cm="1">
         <f t="array" aca="1" ref="AM23" ca="1">MY_BIN2HEX(AJ23)</f>
@@ -4030,6 +4086,22 @@
       <c r="AG24" s="18">
         <v>0</v>
       </c>
+      <c r="AH24" s="22" t="str">
+        <f t="shared" si="17"/>
+        <v>0000000000</v>
+      </c>
+      <c r="AI24" s="22" t="str">
+        <f t="shared" si="18"/>
+        <v>0110000000</v>
+      </c>
+      <c r="AJ24" s="22" t="str">
+        <f t="shared" si="19"/>
+        <v>00000000000110000000</v>
+      </c>
+      <c r="AK24" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>***011000010</v>
+      </c>
     </row>
     <row r="25" spans="1:39" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
@@ -4131,6 +4203,22 @@
       <c r="AG25" s="18">
         <v>1</v>
       </c>
+      <c r="AH25" s="22" t="str">
+        <f t="shared" si="17"/>
+        <v>0000000010</v>
+      </c>
+      <c r="AI25" s="22" t="str">
+        <f t="shared" si="18"/>
+        <v>0000011011</v>
+      </c>
+      <c r="AJ25" s="22" t="str">
+        <f t="shared" si="19"/>
+        <v>00000000100000011011</v>
+      </c>
+      <c r="AK25" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>***011000011</v>
+      </c>
     </row>
     <row r="26" spans="1:39" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
@@ -4232,6 +4320,22 @@
       <c r="AG26" s="18">
         <v>1</v>
       </c>
+      <c r="AH26" s="22" t="str">
+        <f t="shared" si="17"/>
+        <v>0001000000</v>
+      </c>
+      <c r="AI26" s="22" t="str">
+        <f t="shared" si="18"/>
+        <v>0100000001</v>
+      </c>
+      <c r="AJ26" s="22" t="str">
+        <f t="shared" si="19"/>
+        <v>00010000000100000001</v>
+      </c>
+      <c r="AK26" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>*1*011010011</v>
+      </c>
     </row>
     <row r="27" spans="1:39" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
@@ -4333,6 +4437,22 @@
       <c r="AG27" s="18">
         <v>1</v>
       </c>
+      <c r="AH27" s="22" t="str">
+        <f t="shared" si="17"/>
+        <v>0001000000</v>
+      </c>
+      <c r="AI27" s="22" t="str">
+        <f t="shared" si="18"/>
+        <v>0100000001</v>
+      </c>
+      <c r="AJ27" s="22" t="str">
+        <f t="shared" si="19"/>
+        <v>00010000000100000001</v>
+      </c>
+      <c r="AK27" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>**1011100011</v>
+      </c>
     </row>
     <row r="28" spans="1:39" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
@@ -4434,8 +4554,27 @@
       <c r="AG28" s="18">
         <v>1</v>
       </c>
+      <c r="AH28" s="22" t="str">
+        <f t="shared" si="17"/>
+        <v>0001000000</v>
+      </c>
+      <c r="AI28" s="22" t="str">
+        <f t="shared" si="18"/>
+        <v>0100000001</v>
+      </c>
+      <c r="AJ28" s="22" t="str">
+        <f t="shared" si="19"/>
+        <v>00010000000100000001</v>
+      </c>
+      <c r="AK28" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>1**011110011</v>
+      </c>
     </row>
-    <row r="37" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="14:36" x14ac:dyDescent="0.25">
+      <c r="AJ33" s="45"/>
+    </row>
+    <row r="37" spans="14:36" x14ac:dyDescent="0.25">
       <c r="N37" s="45"/>
     </row>
   </sheetData>

</xml_diff>